<commit_message>
updated readme with Windows instructions AND added data file delete to script
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="26 JAN 2026" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="27 JAN 2026" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -5895,4 +5896,4921 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G148"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="8" customWidth="1" min="1" max="1"/>
+    <col width="9" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="9" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="26" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Close $</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Beta</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>RSI</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>MACD</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Signal</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Avg $ Vol</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr"/>
+      <c r="B2" s="2" t="inlineStr"/>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>252 days
+&gt; 1.2</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>14 days
+50.0 to 70.0</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>12/26 EMA
+MACD &gt; Signal</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>12 days</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>6 months
+&gt; $5,000,000</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="17" customHeight="1">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>ADNT</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>22.23</v>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>1.37</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>59.32</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>0.63</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>0.51</t>
+        </is>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>24889782.54905512</v>
+      </c>
+    </row>
+    <row r="4" ht="17" customHeight="1">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>AESI</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>11.61</v>
+      </c>
+      <c r="C4" s="7" t="inlineStr">
+        <is>
+          <t>1.47</t>
+        </is>
+      </c>
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t>67.09</t>
+        </is>
+      </c>
+      <c r="E4" s="7" t="inlineStr">
+        <is>
+          <t>0.52</t>
+        </is>
+      </c>
+      <c r="F4" s="7" t="inlineStr">
+        <is>
+          <t>0.36</t>
+        </is>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>25565786.28771653</v>
+      </c>
+    </row>
+    <row r="5" ht="17" customHeight="1">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>AGX</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>362.58</v>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>1.56</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>55.99</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>11.17</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>6.39</t>
+        </is>
+      </c>
+      <c r="G5" s="4" t="n">
+        <v>106840351.3944882</v>
+      </c>
+    </row>
+    <row r="6" ht="17" customHeight="1">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>AMPX</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>11.58</v>
+      </c>
+      <c r="C6" s="7" t="inlineStr">
+        <is>
+          <t>2.54</t>
+        </is>
+      </c>
+      <c r="D6" s="7" t="inlineStr">
+        <is>
+          <t>60.69</t>
+        </is>
+      </c>
+      <c r="E6" s="7" t="inlineStr">
+        <is>
+          <t>0.42</t>
+        </is>
+      </c>
+      <c r="F6" s="7" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>81870805.40582679</v>
+      </c>
+    </row>
+    <row r="7" ht="17" customHeight="1">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>AMRC</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>33.02</v>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>1.58</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>57.30</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>-0.12</t>
+        </is>
+      </c>
+      <c r="G7" s="4" t="n">
+        <v>19320681.19141732</v>
+      </c>
+    </row>
+    <row r="8" ht="17" customHeight="1">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>ANET</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>146.69</v>
+      </c>
+      <c r="C8" s="7" t="inlineStr">
+        <is>
+          <t>1.66</t>
+        </is>
+      </c>
+      <c r="D8" s="7" t="inlineStr">
+        <is>
+          <t>65.85</t>
+        </is>
+      </c>
+      <c r="E8" s="7" t="inlineStr">
+        <is>
+          <t>2.52</t>
+        </is>
+      </c>
+      <c r="F8" s="7" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>1155091679.811181</v>
+      </c>
+    </row>
+    <row r="9" ht="17" customHeight="1">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>ARTY</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>53.55</v>
+      </c>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>1.45</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="inlineStr">
+        <is>
+          <t>69.64</t>
+        </is>
+      </c>
+      <c r="E9" s="5" t="inlineStr">
+        <is>
+          <t>1.04</t>
+        </is>
+      </c>
+      <c r="F9" s="5" t="inlineStr">
+        <is>
+          <t>0.78</t>
+        </is>
+      </c>
+      <c r="G9" s="4" t="n">
+        <v>24523294.84204724</v>
+      </c>
+    </row>
+    <row r="10" ht="17" customHeight="1">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>ASPN</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="C10" s="7" t="inlineStr">
+        <is>
+          <t>1.58</t>
+        </is>
+      </c>
+      <c r="D10" s="7" t="inlineStr">
+        <is>
+          <t>52.95</t>
+        </is>
+      </c>
+      <c r="E10" s="7" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="F10" s="7" t="inlineStr">
+        <is>
+          <t>-0.02</t>
+        </is>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>12199084.30448819</v>
+      </c>
+    </row>
+    <row r="11" ht="17" customHeight="1">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>ATKR</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>70.77</v>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>1.38</t>
+        </is>
+      </c>
+      <c r="D11" s="5" t="inlineStr">
+        <is>
+          <t>57.67</t>
+        </is>
+      </c>
+      <c r="E11" s="5" t="inlineStr">
+        <is>
+          <t>1.83</t>
+        </is>
+      </c>
+      <c r="F11" s="5" t="inlineStr">
+        <is>
+          <t>1.46</t>
+        </is>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>34434482.47992127</v>
+      </c>
+    </row>
+    <row r="12" ht="17" customHeight="1">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>ATMU</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="n">
+        <v>56.73</v>
+      </c>
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>1.23</t>
+        </is>
+      </c>
+      <c r="D12" s="7" t="inlineStr">
+        <is>
+          <t>59.96</t>
+        </is>
+      </c>
+      <c r="E12" s="7" t="inlineStr">
+        <is>
+          <t>1.35</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr">
+        <is>
+          <t>1.26</t>
+        </is>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>33004321.306063</v>
+      </c>
+    </row>
+    <row r="13" ht="17" customHeight="1">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>AUB</t>
+        </is>
+      </c>
+      <c r="B13" s="4" t="n">
+        <v>39.32</v>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>1.21</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="inlineStr">
+        <is>
+          <t>63.56</t>
+        </is>
+      </c>
+      <c r="E13" s="5" t="inlineStr">
+        <is>
+          <t>0.96</t>
+        </is>
+      </c>
+      <c r="F13" s="5" t="inlineStr">
+        <is>
+          <t>0.79</t>
+        </is>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>39215677.21133859</v>
+      </c>
+    </row>
+    <row r="14" ht="17" customHeight="1">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>AXL</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="n">
+        <v>8.039999999999999</v>
+      </c>
+      <c r="C14" s="7" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="D14" s="7" t="inlineStr">
+        <is>
+          <t>63.91</t>
+        </is>
+      </c>
+      <c r="E14" s="7" t="inlineStr">
+        <is>
+          <t>0.42</t>
+        </is>
+      </c>
+      <c r="F14" s="7" t="inlineStr">
+        <is>
+          <t>0.36</t>
+        </is>
+      </c>
+      <c r="G14" s="6" t="n">
+        <v>21131596.06685039</v>
+      </c>
+    </row>
+    <row r="15" ht="17" customHeight="1">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>BA</t>
+        </is>
+      </c>
+      <c r="B15" s="4" t="n">
+        <v>244.56</v>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>1.22</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="inlineStr">
+        <is>
+          <t>66.16</t>
+        </is>
+      </c>
+      <c r="E15" s="5" t="inlineStr">
+        <is>
+          <t>10.03</t>
+        </is>
+      </c>
+      <c r="F15" s="5" t="inlineStr">
+        <is>
+          <t>9.78</t>
+        </is>
+      </c>
+      <c r="G15" s="4" t="n">
+        <v>1751136935.910079</v>
+      </c>
+    </row>
+    <row r="16" ht="17" customHeight="1">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>BAI</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="n">
+        <v>35.43</v>
+      </c>
+      <c r="C16" s="7" t="inlineStr">
+        <is>
+          <t>1.50</t>
+        </is>
+      </c>
+      <c r="D16" s="7" t="inlineStr">
+        <is>
+          <t>59.73</t>
+        </is>
+      </c>
+      <c r="E16" s="7" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="F16" s="7" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>81818025.84700787</v>
+      </c>
+    </row>
+    <row r="17" ht="17" customHeight="1">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>BBBY</t>
+        </is>
+      </c>
+      <c r="B17" s="4" t="n">
+        <v>6.64</v>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>2.29</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="inlineStr">
+        <is>
+          <t>50.64</t>
+        </is>
+      </c>
+      <c r="E17" s="5" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="F17" s="5" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="G17" s="4" t="n">
+        <v>18900214.20417323</v>
+      </c>
+    </row>
+    <row r="18" ht="17" customHeight="1">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>BDC</t>
+        </is>
+      </c>
+      <c r="B18" s="6" t="n">
+        <v>117.57</v>
+      </c>
+      <c r="C18" s="7" t="inlineStr">
+        <is>
+          <t>1.35</t>
+        </is>
+      </c>
+      <c r="D18" s="7" t="inlineStr">
+        <is>
+          <t>50.45</t>
+        </is>
+      </c>
+      <c r="E18" s="7" t="inlineStr">
+        <is>
+          <t>-0.12</t>
+        </is>
+      </c>
+      <c r="F18" s="7" t="inlineStr">
+        <is>
+          <t>-0.14</t>
+        </is>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>33259686.27267716</v>
+      </c>
+    </row>
+    <row r="19" ht="17" customHeight="1">
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>BE</t>
+        </is>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>152.31</v>
+      </c>
+      <c r="C19" s="5" t="inlineStr">
+        <is>
+          <t>1.90</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="inlineStr">
+        <is>
+          <t>68.29</t>
+        </is>
+      </c>
+      <c r="E19" s="5" t="inlineStr">
+        <is>
+          <t>12.77</t>
+        </is>
+      </c>
+      <c r="F19" s="5" t="inlineStr">
+        <is>
+          <t>9.82</t>
+        </is>
+      </c>
+      <c r="G19" s="4" t="n">
+        <v>1236184921.804095</v>
+      </c>
+    </row>
+    <row r="20" ht="17" customHeight="1">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>BHE</t>
+        </is>
+      </c>
+      <c r="B20" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="C20" s="7" t="inlineStr">
+        <is>
+          <t>1.28</t>
+        </is>
+      </c>
+      <c r="D20" s="7" t="inlineStr">
+        <is>
+          <t>59.21</t>
+        </is>
+      </c>
+      <c r="E20" s="7" t="inlineStr">
+        <is>
+          <t>1.32</t>
+        </is>
+      </c>
+      <c r="F20" s="7" t="inlineStr">
+        <is>
+          <t>0.96</t>
+        </is>
+      </c>
+      <c r="G20" s="6" t="n">
+        <v>11983315.87826772</v>
+      </c>
+    </row>
+    <row r="21" ht="17" customHeight="1">
+      <c r="A21" s="3" t="inlineStr">
+        <is>
+          <t>BHVN</t>
+        </is>
+      </c>
+      <c r="B21" s="4" t="n">
+        <v>12.67</v>
+      </c>
+      <c r="C21" s="5" t="inlineStr">
+        <is>
+          <t>1.38</t>
+        </is>
+      </c>
+      <c r="D21" s="5" t="inlineStr">
+        <is>
+          <t>55.84</t>
+        </is>
+      </c>
+      <c r="E21" s="5" t="inlineStr">
+        <is>
+          <t>0.59</t>
+        </is>
+      </c>
+      <c r="F21" s="5" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+      <c r="G21" s="4" t="n">
+        <v>39373309.43929134</v>
+      </c>
+    </row>
+    <row r="22" ht="17" customHeight="1">
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>BKU</t>
+        </is>
+      </c>
+      <c r="B22" s="6" t="n">
+        <v>47.61</v>
+      </c>
+      <c r="C22" s="7" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+      <c r="D22" s="7" t="inlineStr">
+        <is>
+          <t>57.86</t>
+        </is>
+      </c>
+      <c r="E22" s="7" t="inlineStr">
+        <is>
+          <t>1.02</t>
+        </is>
+      </c>
+      <c r="F22" s="7" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="G22" s="6" t="n">
+        <v>37754926.56173228</v>
+      </c>
+    </row>
+    <row r="23" ht="17" customHeight="1">
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>BKV</t>
+        </is>
+      </c>
+      <c r="B23" s="4" t="n">
+        <v>28.34</v>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="inlineStr">
+        <is>
+          <t>59.92</t>
+        </is>
+      </c>
+      <c r="E23" s="5" t="inlineStr">
+        <is>
+          <t>0.38</t>
+        </is>
+      </c>
+      <c r="F23" s="5" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="n">
+        <v>15697319.13149606</v>
+      </c>
+    </row>
+    <row r="24" ht="17" customHeight="1">
+      <c r="A24" s="3" t="inlineStr">
+        <is>
+          <t>BORR</t>
+        </is>
+      </c>
+      <c r="B24" s="6" t="n">
+        <v>4.51</v>
+      </c>
+      <c r="C24" s="7" t="inlineStr">
+        <is>
+          <t>1.89</t>
+        </is>
+      </c>
+      <c r="D24" s="7" t="inlineStr">
+        <is>
+          <t>65.77</t>
+        </is>
+      </c>
+      <c r="E24" s="7" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="F24" s="7" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="G24" s="6" t="n">
+        <v>15867366.19149606</v>
+      </c>
+    </row>
+    <row r="25" ht="17" customHeight="1">
+      <c r="A25" s="3" t="inlineStr">
+        <is>
+          <t>CALX</t>
+        </is>
+      </c>
+      <c r="B25" s="4" t="n">
+        <v>55.98</v>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t>1.22</t>
+        </is>
+      </c>
+      <c r="D25" s="5" t="inlineStr">
+        <is>
+          <t>52.69</t>
+        </is>
+      </c>
+      <c r="E25" s="5" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="F25" s="5" t="inlineStr">
+        <is>
+          <t>-0.04</t>
+        </is>
+      </c>
+      <c r="G25" s="4" t="n">
+        <v>39297593.18614175</v>
+      </c>
+    </row>
+    <row r="26" ht="17" customHeight="1">
+      <c r="A26" s="3" t="inlineStr">
+        <is>
+          <t>CALY</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="C26" s="7" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="D26" s="7" t="inlineStr">
+        <is>
+          <t>65.15</t>
+        </is>
+      </c>
+      <c r="E26" s="7" t="inlineStr">
+        <is>
+          <t>0.96</t>
+        </is>
+      </c>
+      <c r="F26" s="7" t="inlineStr">
+        <is>
+          <t>0.84</t>
+        </is>
+      </c>
+      <c r="G26" s="6" t="n">
+        <v>29325609.4703937</v>
+      </c>
+    </row>
+    <row r="27" ht="17" customHeight="1">
+      <c r="A27" s="3" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="B27" s="4" t="n">
+        <v>15.63</v>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
+        <is>
+          <t>2.15</t>
+        </is>
+      </c>
+      <c r="D27" s="5" t="inlineStr">
+        <is>
+          <t>67.20</t>
+        </is>
+      </c>
+      <c r="E27" s="5" t="inlineStr">
+        <is>
+          <t>0.91</t>
+        </is>
+      </c>
+      <c r="F27" s="5" t="inlineStr">
+        <is>
+          <t>0.71</t>
+        </is>
+      </c>
+      <c r="G27" s="4" t="n">
+        <v>42754007.49110237</v>
+      </c>
+    </row>
+    <row r="28" ht="17" customHeight="1">
+      <c r="A28" s="3" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="B28" s="6" t="n">
+        <v>46.86</v>
+      </c>
+      <c r="C28" s="7" t="inlineStr">
+        <is>
+          <t>1.86</t>
+        </is>
+      </c>
+      <c r="D28" s="7" t="inlineStr">
+        <is>
+          <t>58.26</t>
+        </is>
+      </c>
+      <c r="E28" s="7" t="inlineStr">
+        <is>
+          <t>1.44</t>
+        </is>
+      </c>
+      <c r="F28" s="7" t="inlineStr">
+        <is>
+          <t>1.28</t>
+        </is>
+      </c>
+      <c r="G28" s="6" t="n">
+        <v>92730664.63692914</v>
+      </c>
+    </row>
+    <row r="29" ht="17" customHeight="1">
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>CFG</t>
+        </is>
+      </c>
+      <c r="B29" s="4" t="n">
+        <v>63.42</v>
+      </c>
+      <c r="C29" s="5" t="inlineStr">
+        <is>
+          <t>1.23</t>
+        </is>
+      </c>
+      <c r="D29" s="5" t="inlineStr">
+        <is>
+          <t>64.16</t>
+        </is>
+      </c>
+      <c r="E29" s="5" t="inlineStr">
+        <is>
+          <t>1.42</t>
+        </is>
+      </c>
+      <c r="F29" s="5" t="inlineStr">
+        <is>
+          <t>1.34</t>
+        </is>
+      </c>
+      <c r="G29" s="4" t="n">
+        <v>246158776.5120472</v>
+      </c>
+    </row>
+    <row r="30" ht="17" customHeight="1">
+      <c r="A30" s="3" t="inlineStr">
+        <is>
+          <t>CIVI</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="n">
+        <v>27.96</v>
+      </c>
+      <c r="C30" s="7" t="inlineStr">
+        <is>
+          <t>1.90</t>
+        </is>
+      </c>
+      <c r="D30" s="7" t="inlineStr">
+        <is>
+          <t>56.21</t>
+        </is>
+      </c>
+      <c r="E30" s="7" t="inlineStr">
+        <is>
+          <t>-0.09</t>
+        </is>
+      </c>
+      <c r="F30" s="7" t="inlineStr">
+        <is>
+          <t>-0.37</t>
+        </is>
+      </c>
+      <c r="G30" s="6" t="n">
+        <v>66248193.66031495</v>
+      </c>
+    </row>
+    <row r="31" ht="17" customHeight="1">
+      <c r="A31" s="3" t="inlineStr">
+        <is>
+          <t>CLB</t>
+        </is>
+      </c>
+      <c r="B31" s="4" t="n">
+        <v>19.67</v>
+      </c>
+      <c r="C31" s="5" t="inlineStr">
+        <is>
+          <t>1.61</t>
+        </is>
+      </c>
+      <c r="D31" s="5" t="inlineStr">
+        <is>
+          <t>66.00</t>
+        </is>
+      </c>
+      <c r="E31" s="5" t="inlineStr">
+        <is>
+          <t>0.81</t>
+        </is>
+      </c>
+      <c r="F31" s="5" t="inlineStr">
+        <is>
+          <t>0.78</t>
+        </is>
+      </c>
+      <c r="G31" s="4" t="n">
+        <v>6880647.319133859</v>
+      </c>
+    </row>
+    <row r="32" ht="17" customHeight="1">
+      <c r="A32" s="3" t="inlineStr">
+        <is>
+          <t>CLF</t>
+        </is>
+      </c>
+      <c r="B32" s="6" t="n">
+        <v>14.27</v>
+      </c>
+      <c r="C32" s="7" t="inlineStr">
+        <is>
+          <t>2.02</t>
+        </is>
+      </c>
+      <c r="D32" s="7" t="inlineStr">
+        <is>
+          <t>56.34</t>
+        </is>
+      </c>
+      <c r="E32" s="7" t="inlineStr">
+        <is>
+          <t>0.41</t>
+        </is>
+      </c>
+      <c r="F32" s="7" t="inlineStr">
+        <is>
+          <t>0.32</t>
+        </is>
+      </c>
+      <c r="G32" s="6" t="n">
+        <v>269079090.8585827</v>
+      </c>
+    </row>
+    <row r="33" ht="17" customHeight="1">
+      <c r="A33" s="3" t="inlineStr">
+        <is>
+          <t>CLS</t>
+        </is>
+      </c>
+      <c r="B33" s="4" t="n">
+        <v>333.17</v>
+      </c>
+      <c r="C33" s="5" t="inlineStr">
+        <is>
+          <t>2.28</t>
+        </is>
+      </c>
+      <c r="D33" s="5" t="inlineStr">
+        <is>
+          <t>59.18</t>
+        </is>
+      </c>
+      <c r="E33" s="5" t="inlineStr">
+        <is>
+          <t>1.86</t>
+        </is>
+      </c>
+      <c r="F33" s="5" t="inlineStr">
+        <is>
+          <t>-0.04</t>
+        </is>
+      </c>
+      <c r="G33" s="4" t="n">
+        <v>822006597.7392913</v>
+      </c>
+    </row>
+    <row r="34" ht="17" customHeight="1">
+      <c r="A34" s="3" t="inlineStr">
+        <is>
+          <t>CMC</t>
+        </is>
+      </c>
+      <c r="B34" s="6" t="n">
+        <v>76.5</v>
+      </c>
+      <c r="C34" s="7" t="inlineStr">
+        <is>
+          <t>1.23</t>
+        </is>
+      </c>
+      <c r="D34" s="7" t="inlineStr">
+        <is>
+          <t>62.64</t>
+        </is>
+      </c>
+      <c r="E34" s="7" t="inlineStr">
+        <is>
+          <t>2.26</t>
+        </is>
+      </c>
+      <c r="F34" s="7" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="G34" s="6" t="n">
+        <v>69656208.66196848</v>
+      </c>
+    </row>
+    <row r="35" ht="17" customHeight="1">
+      <c r="A35" s="3" t="inlineStr">
+        <is>
+          <t>CMI</t>
+        </is>
+      </c>
+      <c r="B35" s="4" t="n">
+        <v>576.23</v>
+      </c>
+      <c r="C35" s="5" t="inlineStr">
+        <is>
+          <t>1.24</t>
+        </is>
+      </c>
+      <c r="D35" s="5" t="inlineStr">
+        <is>
+          <t>65.24</t>
+        </is>
+      </c>
+      <c r="E35" s="5" t="inlineStr">
+        <is>
+          <t>17.94</t>
+        </is>
+      </c>
+      <c r="F35" s="5" t="inlineStr">
+        <is>
+          <t>17.68</t>
+        </is>
+      </c>
+      <c r="G35" s="4" t="n">
+        <v>401784331.4976378</v>
+      </c>
+    </row>
+    <row r="36" ht="17" customHeight="1">
+      <c r="A36" s="3" t="inlineStr">
+        <is>
+          <t>COHR</t>
+        </is>
+      </c>
+      <c r="B36" s="6" t="n">
+        <v>214</v>
+      </c>
+      <c r="C36" s="7" t="inlineStr">
+        <is>
+          <t>2.50</t>
+        </is>
+      </c>
+      <c r="D36" s="7" t="inlineStr">
+        <is>
+          <t>65.43</t>
+        </is>
+      </c>
+      <c r="E36" s="7" t="inlineStr">
+        <is>
+          <t>6.99</t>
+        </is>
+      </c>
+      <c r="F36" s="7" t="inlineStr">
+        <is>
+          <t>5.97</t>
+        </is>
+      </c>
+      <c r="G36" s="6" t="n">
+        <v>598339634.8572439</v>
+      </c>
+    </row>
+    <row r="37" ht="17" customHeight="1">
+      <c r="A37" s="3" t="inlineStr">
+        <is>
+          <t>CRC</t>
+        </is>
+      </c>
+      <c r="B37" s="4" t="n">
+        <v>50.68</v>
+      </c>
+      <c r="C37" s="5" t="inlineStr">
+        <is>
+          <t>1.28</t>
+        </is>
+      </c>
+      <c r="D37" s="5" t="inlineStr">
+        <is>
+          <t>65.67</t>
+        </is>
+      </c>
+      <c r="E37" s="5" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="F37" s="5" t="inlineStr">
+        <is>
+          <t>0.39</t>
+        </is>
+      </c>
+      <c r="G37" s="4" t="n">
+        <v>46085082.29228347</v>
+      </c>
+    </row>
+    <row r="38" ht="17" customHeight="1">
+      <c r="A38" s="3" t="inlineStr">
+        <is>
+          <t>CRGY</t>
+        </is>
+      </c>
+      <c r="B38" s="6" t="n">
+        <v>9.220000000000001</v>
+      </c>
+      <c r="C38" s="7" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="D38" s="7" t="inlineStr">
+        <is>
+          <t>63.32</t>
+        </is>
+      </c>
+      <c r="E38" s="7" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="F38" s="7" t="inlineStr">
+        <is>
+          <t>-0.09</t>
+        </is>
+      </c>
+      <c r="G38" s="6" t="n">
+        <v>46807627.26976379</v>
+      </c>
+    </row>
+    <row r="39" ht="17" customHeight="1">
+      <c r="A39" s="3" t="inlineStr">
+        <is>
+          <t>CRS</t>
+        </is>
+      </c>
+      <c r="B39" s="4" t="n">
+        <v>348.99</v>
+      </c>
+      <c r="C39" s="5" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="D39" s="5" t="inlineStr">
+        <is>
+          <t>62.08</t>
+        </is>
+      </c>
+      <c r="E39" s="5" t="inlineStr">
+        <is>
+          <t>5.61</t>
+        </is>
+      </c>
+      <c r="F39" s="5" t="inlineStr">
+        <is>
+          <t>4.26</t>
+        </is>
+      </c>
+      <c r="G39" s="4" t="n">
+        <v>258110445.1088189</v>
+      </c>
+    </row>
+    <row r="40" ht="17" customHeight="1">
+      <c r="A40" s="3" t="inlineStr">
+        <is>
+          <t>CSTM</t>
+        </is>
+      </c>
+      <c r="B40" s="6" t="n">
+        <v>22.69</v>
+      </c>
+      <c r="C40" s="7" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="D40" s="7" t="inlineStr">
+        <is>
+          <t>69.96</t>
+        </is>
+      </c>
+      <c r="E40" s="7" t="inlineStr">
+        <is>
+          <t>1.19</t>
+        </is>
+      </c>
+      <c r="F40" s="7" t="inlineStr">
+        <is>
+          <t>1.14</t>
+        </is>
+      </c>
+      <c r="G40" s="6" t="n">
+        <v>21118891.82173229</v>
+      </c>
+    </row>
+    <row r="41" ht="17" customHeight="1">
+      <c r="A41" s="3" t="inlineStr">
+        <is>
+          <t>CTRI</t>
+        </is>
+      </c>
+      <c r="B41" s="4" t="n">
+        <v>28.48</v>
+      </c>
+      <c r="C41" s="5" t="inlineStr">
+        <is>
+          <t>1.31</t>
+        </is>
+      </c>
+      <c r="D41" s="5" t="inlineStr">
+        <is>
+          <t>69.40</t>
+        </is>
+      </c>
+      <c r="E41" s="5" t="inlineStr">
+        <is>
+          <t>0.92</t>
+        </is>
+      </c>
+      <c r="F41" s="5" t="inlineStr">
+        <is>
+          <t>0.84</t>
+        </is>
+      </c>
+      <c r="G41" s="4" t="n">
+        <v>43852914.77999999</v>
+      </c>
+    </row>
+    <row r="42" ht="17" customHeight="1">
+      <c r="A42" s="3" t="inlineStr">
+        <is>
+          <t>CVNA</t>
+        </is>
+      </c>
+      <c r="B42" s="6" t="n">
+        <v>477.72</v>
+      </c>
+      <c r="C42" s="7" t="inlineStr">
+        <is>
+          <t>2.39</t>
+        </is>
+      </c>
+      <c r="D42" s="7" t="inlineStr">
+        <is>
+          <t>62.27</t>
+        </is>
+      </c>
+      <c r="E42" s="7" t="inlineStr">
+        <is>
+          <t>14.00</t>
+        </is>
+      </c>
+      <c r="F42" s="7" t="inlineStr">
+        <is>
+          <t>13.67</t>
+        </is>
+      </c>
+      <c r="G42" s="6" t="n">
+        <v>1319939638.059764</v>
+      </c>
+    </row>
+    <row r="43" ht="17" customHeight="1">
+      <c r="A43" s="3" t="inlineStr">
+        <is>
+          <t>DD</t>
+        </is>
+      </c>
+      <c r="B43" s="4" t="n">
+        <v>44.61</v>
+      </c>
+      <c r="C43" s="5" t="inlineStr">
+        <is>
+          <t>1.34</t>
+        </is>
+      </c>
+      <c r="D43" s="5" t="inlineStr">
+        <is>
+          <t>66.97</t>
+        </is>
+      </c>
+      <c r="E43" s="5" t="inlineStr">
+        <is>
+          <t>0.92</t>
+        </is>
+      </c>
+      <c r="F43" s="5" t="inlineStr">
+        <is>
+          <t>0.88</t>
+        </is>
+      </c>
+      <c r="G43" s="4" t="n">
+        <v>238079672.1712386</v>
+      </c>
+    </row>
+    <row r="44" ht="17" customHeight="1">
+      <c r="A44" s="3" t="inlineStr">
+        <is>
+          <t>DDD</t>
+        </is>
+      </c>
+      <c r="B44" s="6" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="C44" s="7" t="inlineStr">
+        <is>
+          <t>1.81</t>
+        </is>
+      </c>
+      <c r="D44" s="7" t="inlineStr">
+        <is>
+          <t>51.95</t>
+        </is>
+      </c>
+      <c r="E44" s="7" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="F44" s="7" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="G44" s="6" t="n">
+        <v>10060809.10007874</v>
+      </c>
+    </row>
+    <row r="45" ht="17" customHeight="1">
+      <c r="A45" s="3" t="inlineStr">
+        <is>
+          <t>DNA</t>
+        </is>
+      </c>
+      <c r="B45" s="4" t="n">
+        <v>9.710000000000001</v>
+      </c>
+      <c r="C45" s="5" t="inlineStr">
+        <is>
+          <t>1.89</t>
+        </is>
+      </c>
+      <c r="D45" s="5" t="inlineStr">
+        <is>
+          <t>53.13</t>
+        </is>
+      </c>
+      <c r="E45" s="5" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="F45" s="5" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="G45" s="4" t="n">
+        <v>15480369.52370079</v>
+      </c>
+    </row>
+    <row r="46" ht="17" customHeight="1">
+      <c r="A46" s="3" t="inlineStr">
+        <is>
+          <t>DOW</t>
+        </is>
+      </c>
+      <c r="B46" s="6" t="n">
+        <v>27.81</v>
+      </c>
+      <c r="C46" s="7" t="inlineStr">
+        <is>
+          <t>1.45</t>
+        </is>
+      </c>
+      <c r="D46" s="7" t="inlineStr">
+        <is>
+          <t>63.20</t>
+        </is>
+      </c>
+      <c r="E46" s="7" t="inlineStr">
+        <is>
+          <t>1.19</t>
+        </is>
+      </c>
+      <c r="F46" s="7" t="inlineStr">
+        <is>
+          <t>1.01</t>
+        </is>
+      </c>
+      <c r="G46" s="6" t="n">
+        <v>308494028.6724409</v>
+      </c>
+    </row>
+    <row r="47" ht="17" customHeight="1">
+      <c r="A47" s="3" t="inlineStr">
+        <is>
+          <t>DVN</t>
+        </is>
+      </c>
+      <c r="B47" s="4" t="n">
+        <v>39.45</v>
+      </c>
+      <c r="C47" s="5" t="inlineStr">
+        <is>
+          <t>1.27</t>
+        </is>
+      </c>
+      <c r="D47" s="5" t="inlineStr">
+        <is>
+          <t>63.90</t>
+        </is>
+      </c>
+      <c r="E47" s="5" t="inlineStr">
+        <is>
+          <t>0.62</t>
+        </is>
+      </c>
+      <c r="F47" s="5" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="G47" s="4" t="n">
+        <v>277528799.2738582</v>
+      </c>
+    </row>
+    <row r="48" ht="17" customHeight="1">
+      <c r="A48" s="3" t="inlineStr">
+        <is>
+          <t>ECG</t>
+        </is>
+      </c>
+      <c r="B48" s="6" t="n">
+        <v>93.84999999999999</v>
+      </c>
+      <c r="C48" s="7" t="inlineStr">
+        <is>
+          <t>1.63</t>
+        </is>
+      </c>
+      <c r="D48" s="7" t="inlineStr">
+        <is>
+          <t>57.93</t>
+        </is>
+      </c>
+      <c r="E48" s="7" t="inlineStr">
+        <is>
+          <t>0.87</t>
+        </is>
+      </c>
+      <c r="F48" s="7" t="inlineStr">
+        <is>
+          <t>0.13</t>
+        </is>
+      </c>
+      <c r="G48" s="6" t="n">
+        <v>46805689.89519685</v>
+      </c>
+    </row>
+    <row r="49" ht="17" customHeight="1">
+      <c r="A49" s="3" t="inlineStr">
+        <is>
+          <t>EFXT</t>
+        </is>
+      </c>
+      <c r="B49" s="4" t="n">
+        <v>17.47</v>
+      </c>
+      <c r="C49" s="5" t="inlineStr">
+        <is>
+          <t>1.29</t>
+        </is>
+      </c>
+      <c r="D49" s="5" t="inlineStr">
+        <is>
+          <t>69.76</t>
+        </is>
+      </c>
+      <c r="E49" s="5" t="inlineStr">
+        <is>
+          <t>0.57</t>
+        </is>
+      </c>
+      <c r="F49" s="5" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="G49" s="4" t="n">
+        <v>5952565.232125985</v>
+      </c>
+    </row>
+    <row r="50" ht="17" customHeight="1">
+      <c r="A50" s="3" t="inlineStr">
+        <is>
+          <t>EL</t>
+        </is>
+      </c>
+      <c r="B50" s="6" t="n">
+        <v>116.44</v>
+      </c>
+      <c r="C50" s="7" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="D50" s="7" t="inlineStr">
+        <is>
+          <t>62.13</t>
+        </is>
+      </c>
+      <c r="E50" s="7" t="inlineStr">
+        <is>
+          <t>3.63</t>
+        </is>
+      </c>
+      <c r="F50" s="7" t="inlineStr">
+        <is>
+          <t>3.58</t>
+        </is>
+      </c>
+      <c r="G50" s="6" t="n">
+        <v>342982740.6979527</v>
+      </c>
+    </row>
+    <row r="51" ht="17" customHeight="1">
+      <c r="A51" s="3" t="inlineStr">
+        <is>
+          <t>ELAN</t>
+        </is>
+      </c>
+      <c r="B51" s="4" t="n">
+        <v>24.62</v>
+      </c>
+      <c r="C51" s="5" t="inlineStr">
+        <is>
+          <t>1.30</t>
+        </is>
+      </c>
+      <c r="D51" s="5" t="inlineStr">
+        <is>
+          <t>61.92</t>
+        </is>
+      </c>
+      <c r="E51" s="5" t="inlineStr">
+        <is>
+          <t>0.61</t>
+        </is>
+      </c>
+      <c r="F51" s="5" t="inlineStr">
+        <is>
+          <t>0.54</t>
+        </is>
+      </c>
+      <c r="G51" s="4" t="n">
+        <v>127602396.2630709</v>
+      </c>
+    </row>
+    <row r="52" ht="17" customHeight="1">
+      <c r="A52" s="3" t="inlineStr">
+        <is>
+          <t>ELF</t>
+        </is>
+      </c>
+      <c r="B52" s="6" t="n">
+        <v>86.73</v>
+      </c>
+      <c r="C52" s="7" t="inlineStr">
+        <is>
+          <t>1.64</t>
+        </is>
+      </c>
+      <c r="D52" s="7" t="inlineStr">
+        <is>
+          <t>51.64</t>
+        </is>
+      </c>
+      <c r="E52" s="7" t="inlineStr">
+        <is>
+          <t>2.45</t>
+        </is>
+      </c>
+      <c r="F52" s="7" t="inlineStr">
+        <is>
+          <t>1.59</t>
+        </is>
+      </c>
+      <c r="G52" s="6" t="n">
+        <v>213983383.1225197</v>
+      </c>
+    </row>
+    <row r="53" ht="17" customHeight="1">
+      <c r="A53" s="3" t="inlineStr">
+        <is>
+          <t>EME</t>
+        </is>
+      </c>
+      <c r="B53" s="4" t="n">
+        <v>716.28</v>
+      </c>
+      <c r="C53" s="5" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="D53" s="5" t="inlineStr">
+        <is>
+          <t>66.66</t>
+        </is>
+      </c>
+      <c r="E53" s="5" t="inlineStr">
+        <is>
+          <t>21.03</t>
+        </is>
+      </c>
+      <c r="F53" s="5" t="inlineStr">
+        <is>
+          <t>14.25</t>
+        </is>
+      </c>
+      <c r="G53" s="4" t="n">
+        <v>318796682.5076379</v>
+      </c>
+    </row>
+    <row r="54" ht="17" customHeight="1">
+      <c r="A54" s="3" t="inlineStr">
+        <is>
+          <t>EMR</t>
+        </is>
+      </c>
+      <c r="B54" s="6" t="n">
+        <v>147.67</v>
+      </c>
+      <c r="C54" s="7" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+      <c r="D54" s="7" t="inlineStr">
+        <is>
+          <t>58.90</t>
+        </is>
+      </c>
+      <c r="E54" s="7" t="inlineStr">
+        <is>
+          <t>3.44</t>
+        </is>
+      </c>
+      <c r="F54" s="7" t="inlineStr">
+        <is>
+          <t>3.24</t>
+        </is>
+      </c>
+      <c r="G54" s="6" t="n">
+        <v>388527433.0128346</v>
+      </c>
+    </row>
+    <row r="55" ht="17" customHeight="1">
+      <c r="A55" s="3" t="inlineStr">
+        <is>
+          <t>ESI</t>
+        </is>
+      </c>
+      <c r="B55" s="4" t="n">
+        <v>29.29</v>
+      </c>
+      <c r="C55" s="5" t="inlineStr">
+        <is>
+          <t>1.46</t>
+        </is>
+      </c>
+      <c r="D55" s="5" t="inlineStr">
+        <is>
+          <t>62.37</t>
+        </is>
+      </c>
+      <c r="E55" s="5" t="inlineStr">
+        <is>
+          <t>0.83</t>
+        </is>
+      </c>
+      <c r="F55" s="5" t="inlineStr">
+        <is>
+          <t>0.68</t>
+        </is>
+      </c>
+      <c r="G55" s="4" t="n">
+        <v>55694922.13031495</v>
+      </c>
+    </row>
+    <row r="56" ht="17" customHeight="1">
+      <c r="A56" s="3" t="inlineStr">
+        <is>
+          <t>ETN</t>
+        </is>
+      </c>
+      <c r="B56" s="6" t="n">
+        <v>341.19</v>
+      </c>
+      <c r="C56" s="7" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="D56" s="7" t="inlineStr">
+        <is>
+          <t>57.16</t>
+        </is>
+      </c>
+      <c r="E56" s="7" t="inlineStr">
+        <is>
+          <t>1.12</t>
+        </is>
+      </c>
+      <c r="F56" s="7" t="inlineStr">
+        <is>
+          <t>-1.09</t>
+        </is>
+      </c>
+      <c r="G56" s="6" t="n">
+        <v>911578593.3076377</v>
+      </c>
+    </row>
+    <row r="57" ht="17" customHeight="1">
+      <c r="A57" s="3" t="inlineStr">
+        <is>
+          <t>FIX</t>
+        </is>
+      </c>
+      <c r="B57" s="4" t="n">
+        <v>1160.38</v>
+      </c>
+      <c r="C57" s="5" t="inlineStr">
+        <is>
+          <t>1.77</t>
+        </is>
+      </c>
+      <c r="D57" s="5" t="inlineStr">
+        <is>
+          <t>68.41</t>
+        </is>
+      </c>
+      <c r="E57" s="5" t="inlineStr">
+        <is>
+          <t>47.27</t>
+        </is>
+      </c>
+      <c r="F57" s="5" t="inlineStr">
+        <is>
+          <t>35.77</t>
+        </is>
+      </c>
+      <c r="G57" s="4" t="n">
+        <v>431725370.5948819</v>
+      </c>
+    </row>
+    <row r="58" ht="17" customHeight="1">
+      <c r="A58" s="3" t="inlineStr">
+        <is>
+          <t>FLOC</t>
+        </is>
+      </c>
+      <c r="B58" s="6" t="n">
+        <v>20.49</v>
+      </c>
+      <c r="C58" s="7" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="D58" s="7" t="inlineStr">
+        <is>
+          <t>63.10</t>
+        </is>
+      </c>
+      <c r="E58" s="7" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+      <c r="F58" s="7" t="inlineStr">
+        <is>
+          <t>0.63</t>
+        </is>
+      </c>
+      <c r="G58" s="6" t="n">
+        <v>5427332.180787402</v>
+      </c>
+    </row>
+    <row r="59" ht="17" customHeight="1">
+      <c r="A59" s="3" t="inlineStr">
+        <is>
+          <t>FLR</t>
+        </is>
+      </c>
+      <c r="B59" s="4" t="n">
+        <v>45.99</v>
+      </c>
+      <c r="C59" s="5" t="inlineStr">
+        <is>
+          <t>1.52</t>
+        </is>
+      </c>
+      <c r="D59" s="5" t="inlineStr">
+        <is>
+          <t>62.27</t>
+        </is>
+      </c>
+      <c r="E59" s="5" t="inlineStr">
+        <is>
+          <t>0.76</t>
+        </is>
+      </c>
+      <c r="F59" s="5" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+      <c r="G59" s="4" t="n">
+        <v>161726684.747559</v>
+      </c>
+    </row>
+    <row r="60" ht="17" customHeight="1">
+      <c r="A60" s="3" t="inlineStr">
+        <is>
+          <t>FLS</t>
+        </is>
+      </c>
+      <c r="B60" s="6" t="n">
+        <v>77.59999999999999</v>
+      </c>
+      <c r="C60" s="7" t="inlineStr">
+        <is>
+          <t>1.52</t>
+        </is>
+      </c>
+      <c r="D60" s="7" t="inlineStr">
+        <is>
+          <t>66.37</t>
+        </is>
+      </c>
+      <c r="E60" s="7" t="inlineStr">
+        <is>
+          <t>2.01</t>
+        </is>
+      </c>
+      <c r="F60" s="7" t="inlineStr">
+        <is>
+          <t>1.68</t>
+        </is>
+      </c>
+      <c r="G60" s="6" t="n">
+        <v>114270036.4940157</v>
+      </c>
+    </row>
+    <row r="61" ht="17" customHeight="1">
+      <c r="A61" s="3" t="inlineStr">
+        <is>
+          <t>FN</t>
+        </is>
+      </c>
+      <c r="B61" s="4" t="n">
+        <v>498.59</v>
+      </c>
+      <c r="C61" s="5" t="inlineStr">
+        <is>
+          <t>1.90</t>
+        </is>
+      </c>
+      <c r="D61" s="5" t="inlineStr">
+        <is>
+          <t>57.11</t>
+        </is>
+      </c>
+      <c r="E61" s="5" t="inlineStr">
+        <is>
+          <t>5.62</t>
+        </is>
+      </c>
+      <c r="F61" s="5" t="inlineStr">
+        <is>
+          <t>5.32</t>
+        </is>
+      </c>
+      <c r="G61" s="4" t="n">
+        <v>260123819.0626771</v>
+      </c>
+    </row>
+    <row r="62" ht="17" customHeight="1">
+      <c r="A62" s="3" t="inlineStr">
+        <is>
+          <t>FND</t>
+        </is>
+      </c>
+      <c r="B62" s="6" t="n">
+        <v>71.84</v>
+      </c>
+      <c r="C62" s="7" t="inlineStr">
+        <is>
+          <t>1.29</t>
+        </is>
+      </c>
+      <c r="D62" s="7" t="inlineStr">
+        <is>
+          <t>54.94</t>
+        </is>
+      </c>
+      <c r="E62" s="7" t="inlineStr">
+        <is>
+          <t>2.67</t>
+        </is>
+      </c>
+      <c r="F62" s="7" t="inlineStr">
+        <is>
+          <t>2.58</t>
+        </is>
+      </c>
+      <c r="G62" s="6" t="n">
+        <v>170906513.5196063</v>
+      </c>
+    </row>
+    <row r="63" ht="17" customHeight="1">
+      <c r="A63" s="3" t="inlineStr">
+        <is>
+          <t>FUN</t>
+        </is>
+      </c>
+      <c r="B63" s="4" t="n">
+        <v>17.47</v>
+      </c>
+      <c r="C63" s="5" t="inlineStr">
+        <is>
+          <t>1.58</t>
+        </is>
+      </c>
+      <c r="D63" s="5" t="inlineStr">
+        <is>
+          <t>59.42</t>
+        </is>
+      </c>
+      <c r="E63" s="5" t="inlineStr">
+        <is>
+          <t>0.60</t>
+        </is>
+      </c>
+      <c r="F63" s="5" t="inlineStr">
+        <is>
+          <t>0.26</t>
+        </is>
+      </c>
+      <c r="G63" s="4" t="n">
+        <v>83610715.25322835</v>
+      </c>
+    </row>
+    <row r="64" ht="17" customHeight="1">
+      <c r="A64" s="3" t="inlineStr">
+        <is>
+          <t>GARP</t>
+        </is>
+      </c>
+      <c r="B64" s="6" t="n">
+        <v>70.89</v>
+      </c>
+      <c r="C64" s="7" t="inlineStr">
+        <is>
+          <t>1.24</t>
+        </is>
+      </c>
+      <c r="D64" s="7" t="inlineStr">
+        <is>
+          <t>61.81</t>
+        </is>
+      </c>
+      <c r="E64" s="7" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="F64" s="7" t="inlineStr">
+        <is>
+          <t>0.41</t>
+        </is>
+      </c>
+      <c r="G64" s="6" t="n">
+        <v>14643185.6924441</v>
+      </c>
+    </row>
+    <row r="65" ht="17" customHeight="1">
+      <c r="A65" s="3" t="inlineStr">
+        <is>
+          <t>GCO</t>
+        </is>
+      </c>
+      <c r="B65" s="4" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="C65" s="5" t="inlineStr">
+        <is>
+          <t>1.88</t>
+        </is>
+      </c>
+      <c r="D65" s="5" t="inlineStr">
+        <is>
+          <t>52.64</t>
+        </is>
+      </c>
+      <c r="E65" s="5" t="inlineStr">
+        <is>
+          <t>2.03</t>
+        </is>
+      </c>
+      <c r="F65" s="5" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="G65" s="4" t="n">
+        <v>5281035.736771652</v>
+      </c>
+    </row>
+    <row r="66" ht="17" customHeight="1">
+      <c r="A66" s="3" t="inlineStr">
+        <is>
+          <t>GEV</t>
+        </is>
+      </c>
+      <c r="B66" s="6" t="n">
+        <v>692.7</v>
+      </c>
+      <c r="C66" s="7" t="inlineStr">
+        <is>
+          <t>1.73</t>
+        </is>
+      </c>
+      <c r="D66" s="7" t="inlineStr">
+        <is>
+          <t>59.72</t>
+        </is>
+      </c>
+      <c r="E66" s="7" t="inlineStr">
+        <is>
+          <t>8.29</t>
+        </is>
+      </c>
+      <c r="F66" s="7" t="inlineStr">
+        <is>
+          <t>7.71</t>
+        </is>
+      </c>
+      <c r="G66" s="6" t="n">
+        <v>1869436533.703701</v>
+      </c>
+    </row>
+    <row r="67" ht="17" customHeight="1">
+      <c r="A67" s="3" t="inlineStr">
+        <is>
+          <t>GKOS</t>
+        </is>
+      </c>
+      <c r="B67" s="4" t="n">
+        <v>118.7</v>
+      </c>
+      <c r="C67" s="5" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="D67" s="5" t="inlineStr">
+        <is>
+          <t>54.68</t>
+        </is>
+      </c>
+      <c r="E67" s="5" t="inlineStr">
+        <is>
+          <t>3.52</t>
+        </is>
+      </c>
+      <c r="F67" s="5" t="inlineStr">
+        <is>
+          <t>3.15</t>
+        </is>
+      </c>
+      <c r="G67" s="4" t="n">
+        <v>94658444.54165353</v>
+      </c>
+    </row>
+    <row r="68" ht="17" customHeight="1">
+      <c r="A68" s="3" t="inlineStr">
+        <is>
+          <t>GLOB</t>
+        </is>
+      </c>
+      <c r="B68" s="6" t="n">
+        <v>69.15000000000001</v>
+      </c>
+      <c r="C68" s="7" t="inlineStr">
+        <is>
+          <t>1.54</t>
+        </is>
+      </c>
+      <c r="D68" s="7" t="inlineStr">
+        <is>
+          <t>54.58</t>
+        </is>
+      </c>
+      <c r="E68" s="7" t="inlineStr">
+        <is>
+          <t>0.54</t>
+        </is>
+      </c>
+      <c r="F68" s="7" t="inlineStr">
+        <is>
+          <t>0.46</t>
+        </is>
+      </c>
+      <c r="G68" s="6" t="n">
+        <v>94382873.52440949</v>
+      </c>
+    </row>
+    <row r="69" ht="17" customHeight="1">
+      <c r="A69" s="3" t="inlineStr">
+        <is>
+          <t>GNRC</t>
+        </is>
+      </c>
+      <c r="B69" s="4" t="n">
+        <v>170.45</v>
+      </c>
+      <c r="C69" s="5" t="inlineStr">
+        <is>
+          <t>1.34</t>
+        </is>
+      </c>
+      <c r="D69" s="5" t="inlineStr">
+        <is>
+          <t>63.27</t>
+        </is>
+      </c>
+      <c r="E69" s="5" t="inlineStr">
+        <is>
+          <t>5.70</t>
+        </is>
+      </c>
+      <c r="F69" s="5" t="inlineStr">
+        <is>
+          <t>2.68</t>
+        </is>
+      </c>
+      <c r="G69" s="4" t="n">
+        <v>191080402.5101575</v>
+      </c>
+    </row>
+    <row r="70" ht="17" customHeight="1">
+      <c r="A70" s="3" t="inlineStr">
+        <is>
+          <t>GRNY</t>
+        </is>
+      </c>
+      <c r="B70" s="6" t="n">
+        <v>25.85</v>
+      </c>
+      <c r="C70" s="7" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+      <c r="D70" s="7" t="inlineStr">
+        <is>
+          <t>58.01</t>
+        </is>
+      </c>
+      <c r="E70" s="7" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="F70" s="7" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="G70" s="6" t="n">
+        <v>91699107.17244093</v>
+      </c>
+    </row>
+    <row r="71" ht="17" customHeight="1">
+      <c r="A71" s="3" t="inlineStr">
+        <is>
+          <t>GTES</t>
+        </is>
+      </c>
+      <c r="B71" s="4" t="n">
+        <v>22.72</v>
+      </c>
+      <c r="C71" s="5" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+      <c r="D71" s="5" t="inlineStr">
+        <is>
+          <t>51.31</t>
+        </is>
+      </c>
+      <c r="E71" s="5" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="F71" s="5" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="G71" s="4" t="n">
+        <v>53292090.08417323</v>
+      </c>
+    </row>
+    <row r="72" ht="17" customHeight="1">
+      <c r="A72" s="3" t="inlineStr">
+        <is>
+          <t>HLIO</t>
+        </is>
+      </c>
+      <c r="B72" s="6" t="n">
+        <v>65.81999999999999</v>
+      </c>
+      <c r="C72" s="7" t="inlineStr">
+        <is>
+          <t>1.38</t>
+        </is>
+      </c>
+      <c r="D72" s="7" t="inlineStr">
+        <is>
+          <t>69.54</t>
+        </is>
+      </c>
+      <c r="E72" s="7" t="inlineStr">
+        <is>
+          <t>2.92</t>
+        </is>
+      </c>
+      <c r="F72" s="7" t="inlineStr">
+        <is>
+          <t>2.27</t>
+        </is>
+      </c>
+      <c r="G72" s="6" t="n">
+        <v>17035912.00267716</v>
+      </c>
+    </row>
+    <row r="73" ht="17" customHeight="1">
+      <c r="A73" s="3" t="inlineStr">
+        <is>
+          <t>HLX</t>
+        </is>
+      </c>
+      <c r="B73" s="4" t="n">
+        <v>7.65</v>
+      </c>
+      <c r="C73" s="5" t="inlineStr">
+        <is>
+          <t>1.35</t>
+        </is>
+      </c>
+      <c r="D73" s="5" t="inlineStr">
+        <is>
+          <t>65.81</t>
+        </is>
+      </c>
+      <c r="E73" s="5" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="F73" s="5" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="G73" s="4" t="n">
+        <v>9859916.12015748</v>
+      </c>
+    </row>
+    <row r="74" ht="17" customHeight="1">
+      <c r="A74" s="3" t="inlineStr">
+        <is>
+          <t>HP</t>
+        </is>
+      </c>
+      <c r="B74" s="6" t="n">
+        <v>33.32</v>
+      </c>
+      <c r="C74" s="7" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
+      <c r="D74" s="7" t="inlineStr">
+        <is>
+          <t>67.18</t>
+        </is>
+      </c>
+      <c r="E74" s="7" t="inlineStr">
+        <is>
+          <t>1.10</t>
+        </is>
+      </c>
+      <c r="F74" s="7" t="inlineStr">
+        <is>
+          <t>0.97</t>
+        </is>
+      </c>
+      <c r="G74" s="6" t="n">
+        <v>41467546.26992127</v>
+      </c>
+    </row>
+    <row r="75" ht="17" customHeight="1">
+      <c r="A75" s="3" t="inlineStr">
+        <is>
+          <t>HZO</t>
+        </is>
+      </c>
+      <c r="B75" s="4" t="n">
+        <v>27.56</v>
+      </c>
+      <c r="C75" s="5" t="inlineStr">
+        <is>
+          <t>1.66</t>
+        </is>
+      </c>
+      <c r="D75" s="5" t="inlineStr">
+        <is>
+          <t>55.37</t>
+        </is>
+      </c>
+      <c r="E75" s="5" t="inlineStr">
+        <is>
+          <t>0.87</t>
+        </is>
+      </c>
+      <c r="F75" s="5" t="inlineStr">
+        <is>
+          <t>0.84</t>
+        </is>
+      </c>
+      <c r="G75" s="4" t="n">
+        <v>8317024.592755905</v>
+      </c>
+    </row>
+    <row r="76" ht="17" customHeight="1">
+      <c r="A76" s="3" t="inlineStr">
+        <is>
+          <t>INVX</t>
+        </is>
+      </c>
+      <c r="B76" s="6" t="n">
+        <v>26.09</v>
+      </c>
+      <c r="C76" s="7" t="inlineStr">
+        <is>
+          <t>1.26</t>
+        </is>
+      </c>
+      <c r="D76" s="7" t="inlineStr">
+        <is>
+          <t>69.50</t>
+        </is>
+      </c>
+      <c r="E76" s="7" t="inlineStr">
+        <is>
+          <t>0.90</t>
+        </is>
+      </c>
+      <c r="F76" s="7" t="inlineStr">
+        <is>
+          <t>0.66</t>
+        </is>
+      </c>
+      <c r="G76" s="6" t="n">
+        <v>7291505.044015748</v>
+      </c>
+    </row>
+    <row r="77" ht="17" customHeight="1">
+      <c r="A77" s="3" t="inlineStr">
+        <is>
+          <t>ITT</t>
+        </is>
+      </c>
+      <c r="B77" s="4" t="n">
+        <v>182.96</v>
+      </c>
+      <c r="C77" s="5" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+      <c r="D77" s="5" t="inlineStr">
+        <is>
+          <t>54.18</t>
+        </is>
+      </c>
+      <c r="E77" s="5" t="inlineStr">
+        <is>
+          <t>1.54</t>
+        </is>
+      </c>
+      <c r="F77" s="5" t="inlineStr">
+        <is>
+          <t>1.10</t>
+        </is>
+      </c>
+      <c r="G77" s="4" t="n">
+        <v>108169382.9765355</v>
+      </c>
+    </row>
+    <row r="78" ht="17" customHeight="1">
+      <c r="A78" s="3" t="inlineStr">
+        <is>
+          <t>JBL</t>
+        </is>
+      </c>
+      <c r="B78" s="6" t="n">
+        <v>242.28</v>
+      </c>
+      <c r="C78" s="7" t="inlineStr">
+        <is>
+          <t>1.44</t>
+        </is>
+      </c>
+      <c r="D78" s="7" t="inlineStr">
+        <is>
+          <t>55.97</t>
+        </is>
+      </c>
+      <c r="E78" s="7" t="inlineStr">
+        <is>
+          <t>5.87</t>
+        </is>
+      </c>
+      <c r="F78" s="7" t="inlineStr">
+        <is>
+          <t>5.77</t>
+        </is>
+      </c>
+      <c r="G78" s="6" t="n">
+        <v>287628356.4244094</v>
+      </c>
+    </row>
+    <row r="79" ht="17" customHeight="1">
+      <c r="A79" s="3" t="inlineStr">
+        <is>
+          <t>KAI</t>
+        </is>
+      </c>
+      <c r="B79" s="4" t="n">
+        <v>319.94</v>
+      </c>
+      <c r="C79" s="5" t="inlineStr">
+        <is>
+          <t>1.34</t>
+        </is>
+      </c>
+      <c r="D79" s="5" t="inlineStr">
+        <is>
+          <t>58.48</t>
+        </is>
+      </c>
+      <c r="E79" s="5" t="inlineStr">
+        <is>
+          <t>9.00</t>
+        </is>
+      </c>
+      <c r="F79" s="5" t="inlineStr">
+        <is>
+          <t>8.42</t>
+        </is>
+      </c>
+      <c r="G79" s="4" t="n">
+        <v>39933381.30952755</v>
+      </c>
+    </row>
+    <row r="80" ht="17" customHeight="1">
+      <c r="A80" s="3" t="inlineStr">
+        <is>
+          <t>KMX</t>
+        </is>
+      </c>
+      <c r="B80" s="6" t="n">
+        <v>46.34</v>
+      </c>
+      <c r="C80" s="7" t="inlineStr">
+        <is>
+          <t>1.21</t>
+        </is>
+      </c>
+      <c r="D80" s="7" t="inlineStr">
+        <is>
+          <t>58.99</t>
+        </is>
+      </c>
+      <c r="E80" s="7" t="inlineStr">
+        <is>
+          <t>1.88</t>
+        </is>
+      </c>
+      <c r="F80" s="7" t="inlineStr">
+        <is>
+          <t>1.81</t>
+        </is>
+      </c>
+      <c r="G80" s="6" t="n">
+        <v>200042012.6100787</v>
+      </c>
+    </row>
+    <row r="81" ht="17" customHeight="1">
+      <c r="A81" s="3" t="inlineStr">
+        <is>
+          <t>KN</t>
+        </is>
+      </c>
+      <c r="B81" s="4" t="n">
+        <v>24.23</v>
+      </c>
+      <c r="C81" s="5" t="inlineStr">
+        <is>
+          <t>1.44</t>
+        </is>
+      </c>
+      <c r="D81" s="5" t="inlineStr">
+        <is>
+          <t>57.60</t>
+        </is>
+      </c>
+      <c r="E81" s="5" t="inlineStr">
+        <is>
+          <t>0.52</t>
+        </is>
+      </c>
+      <c r="F81" s="5" t="inlineStr">
+        <is>
+          <t>0.39</t>
+        </is>
+      </c>
+      <c r="G81" s="4" t="n">
+        <v>15195500.82519685</v>
+      </c>
+    </row>
+    <row r="82" ht="17" customHeight="1">
+      <c r="A82" s="3" t="inlineStr">
+        <is>
+          <t>KOS</t>
+        </is>
+      </c>
+      <c r="B82" s="6" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="C82" s="7" t="inlineStr">
+        <is>
+          <t>1.76</t>
+        </is>
+      </c>
+      <c r="D82" s="7" t="inlineStr">
+        <is>
+          <t>68.63</t>
+        </is>
+      </c>
+      <c r="E82" s="7" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="F82" s="7" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="G82" s="6" t="n">
+        <v>17177972.44423543</v>
+      </c>
+    </row>
+    <row r="83" ht="17" customHeight="1">
+      <c r="A83" s="3" t="inlineStr">
+        <is>
+          <t>LAZ</t>
+        </is>
+      </c>
+      <c r="B83" s="4" t="n">
+        <v>52.77</v>
+      </c>
+      <c r="C83" s="5" t="inlineStr">
+        <is>
+          <t>1.71</t>
+        </is>
+      </c>
+      <c r="D83" s="5" t="inlineStr">
+        <is>
+          <t>54.98</t>
+        </is>
+      </c>
+      <c r="E83" s="5" t="inlineStr">
+        <is>
+          <t>0.62</t>
+        </is>
+      </c>
+      <c r="F83" s="5" t="inlineStr">
+        <is>
+          <t>0.51</t>
+        </is>
+      </c>
+      <c r="G83" s="4" t="n">
+        <v>45832958.77858268</v>
+      </c>
+    </row>
+    <row r="84" ht="17" customHeight="1">
+      <c r="A84" s="3" t="inlineStr">
+        <is>
+          <t>LB</t>
+        </is>
+      </c>
+      <c r="B84" s="6" t="n">
+        <v>56.42</v>
+      </c>
+      <c r="C84" s="7" t="inlineStr">
+        <is>
+          <t>1.74</t>
+        </is>
+      </c>
+      <c r="D84" s="7" t="inlineStr">
+        <is>
+          <t>52.36</t>
+        </is>
+      </c>
+      <c r="E84" s="7" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+      <c r="F84" s="7" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="G84" s="6" t="n">
+        <v>26074278.65472441</v>
+      </c>
+    </row>
+    <row r="85" ht="17" customHeight="1">
+      <c r="A85" s="3" t="inlineStr">
+        <is>
+          <t>LC</t>
+        </is>
+      </c>
+      <c r="B85" s="4" t="n">
+        <v>20.81</v>
+      </c>
+      <c r="C85" s="5" t="inlineStr">
+        <is>
+          <t>1.88</t>
+        </is>
+      </c>
+      <c r="D85" s="5" t="inlineStr">
+        <is>
+          <t>56.21</t>
+        </is>
+      </c>
+      <c r="E85" s="5" t="inlineStr">
+        <is>
+          <t>0.51</t>
+        </is>
+      </c>
+      <c r="F85" s="5" t="inlineStr">
+        <is>
+          <t>0.46</t>
+        </is>
+      </c>
+      <c r="G85" s="4" t="n">
+        <v>32233233.86330708</v>
+      </c>
+    </row>
+    <row r="86" ht="17" customHeight="1">
+      <c r="A86" s="3" t="inlineStr">
+        <is>
+          <t>LMND</t>
+        </is>
+      </c>
+      <c r="B86" s="6" t="n">
+        <v>87.75</v>
+      </c>
+      <c r="C86" s="7" t="inlineStr">
+        <is>
+          <t>2.11</t>
+        </is>
+      </c>
+      <c r="D86" s="7" t="inlineStr">
+        <is>
+          <t>57.08</t>
+        </is>
+      </c>
+      <c r="E86" s="7" t="inlineStr">
+        <is>
+          <t>3.54</t>
+        </is>
+      </c>
+      <c r="F86" s="7" t="inlineStr">
+        <is>
+          <t>2.50</t>
+        </is>
+      </c>
+      <c r="G86" s="6" t="n">
+        <v>172287113.3395276</v>
+      </c>
+    </row>
+    <row r="87" ht="17" customHeight="1">
+      <c r="A87" s="3" t="inlineStr">
+        <is>
+          <t>LUMN</t>
+        </is>
+      </c>
+      <c r="B87" s="4" t="n">
+        <v>9.289999999999999</v>
+      </c>
+      <c r="C87" s="5" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
+      <c r="D87" s="5" t="inlineStr">
+        <is>
+          <t>62.43</t>
+        </is>
+      </c>
+      <c r="E87" s="5" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="F87" s="5" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="G87" s="4" t="n">
+        <v>120680023.0343307</v>
+      </c>
+    </row>
+    <row r="88" ht="17" customHeight="1">
+      <c r="A88" s="3" t="inlineStr">
+        <is>
+          <t>LYB</t>
+        </is>
+      </c>
+      <c r="B88" s="6" t="n">
+        <v>50.43</v>
+      </c>
+      <c r="C88" s="7" t="inlineStr">
+        <is>
+          <t>1.27</t>
+        </is>
+      </c>
+      <c r="D88" s="7" t="inlineStr">
+        <is>
+          <t>59.35</t>
+        </is>
+      </c>
+      <c r="E88" s="7" t="inlineStr">
+        <is>
+          <t>1.71</t>
+        </is>
+      </c>
+      <c r="F88" s="7" t="inlineStr">
+        <is>
+          <t>1.35</t>
+        </is>
+      </c>
+      <c r="G88" s="6" t="n">
+        <v>254900972.488189</v>
+      </c>
+    </row>
+    <row r="89" ht="17" customHeight="1">
+      <c r="A89" s="3" t="inlineStr">
+        <is>
+          <t>MOD</t>
+        </is>
+      </c>
+      <c r="B89" s="4" t="n">
+        <v>146.9</v>
+      </c>
+      <c r="C89" s="5" t="inlineStr">
+        <is>
+          <t>2.07</t>
+        </is>
+      </c>
+      <c r="D89" s="5" t="inlineStr">
+        <is>
+          <t>58.51</t>
+        </is>
+      </c>
+      <c r="E89" s="5" t="inlineStr">
+        <is>
+          <t>1.40</t>
+        </is>
+      </c>
+      <c r="F89" s="5" t="inlineStr">
+        <is>
+          <t>-1.93</t>
+        </is>
+      </c>
+      <c r="G89" s="4" t="n">
+        <v>153983359.3240157</v>
+      </c>
+    </row>
+    <row r="90" ht="17" customHeight="1">
+      <c r="A90" s="3" t="inlineStr">
+        <is>
+          <t>MTDR</t>
+        </is>
+      </c>
+      <c r="B90" s="6" t="n">
+        <v>43.34</v>
+      </c>
+      <c r="C90" s="7" t="inlineStr">
+        <is>
+          <t>1.41</t>
+        </is>
+      </c>
+      <c r="D90" s="7" t="inlineStr">
+        <is>
+          <t>54.08</t>
+        </is>
+      </c>
+      <c r="E90" s="7" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+      <c r="F90" s="7" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="G90" s="6" t="n">
+        <v>75773128.36047246</v>
+      </c>
+    </row>
+    <row r="91" ht="17" customHeight="1">
+      <c r="A91" s="3" t="inlineStr">
+        <is>
+          <t>MTZ</t>
+        </is>
+      </c>
+      <c r="B91" s="4" t="n">
+        <v>248.59</v>
+      </c>
+      <c r="C91" s="5" t="inlineStr">
+        <is>
+          <t>1.61</t>
+        </is>
+      </c>
+      <c r="D91" s="5" t="inlineStr">
+        <is>
+          <t>67.32</t>
+        </is>
+      </c>
+      <c r="E91" s="5" t="inlineStr">
+        <is>
+          <t>7.14</t>
+        </is>
+      </c>
+      <c r="F91" s="5" t="inlineStr">
+        <is>
+          <t>5.50</t>
+        </is>
+      </c>
+      <c r="G91" s="4" t="n">
+        <v>187891750.2670079</v>
+      </c>
+    </row>
+    <row r="92" ht="17" customHeight="1">
+      <c r="A92" s="3" t="inlineStr">
+        <is>
+          <t>NET</t>
+        </is>
+      </c>
+      <c r="B92" s="6" t="n">
+        <v>205.95</v>
+      </c>
+      <c r="C92" s="7" t="inlineStr">
+        <is>
+          <t>1.64</t>
+        </is>
+      </c>
+      <c r="D92" s="7" t="inlineStr">
+        <is>
+          <t>61.06</t>
+        </is>
+      </c>
+      <c r="E92" s="7" t="inlineStr">
+        <is>
+          <t>-3.89</t>
+        </is>
+      </c>
+      <c r="F92" s="7" t="inlineStr">
+        <is>
+          <t>-5.12</t>
+        </is>
+      </c>
+      <c r="G92" s="6" t="n">
+        <v>566680771.5837797</v>
+      </c>
+    </row>
+    <row r="93" ht="17" customHeight="1">
+      <c r="A93" s="3" t="inlineStr">
+        <is>
+          <t>NGVT</t>
+        </is>
+      </c>
+      <c r="B93" s="4" t="n">
+        <v>66.88</v>
+      </c>
+      <c r="C93" s="5" t="inlineStr">
+        <is>
+          <t>1.41</t>
+        </is>
+      </c>
+      <c r="D93" s="5" t="inlineStr">
+        <is>
+          <t>62.33</t>
+        </is>
+      </c>
+      <c r="E93" s="5" t="inlineStr">
+        <is>
+          <t>2.78</t>
+        </is>
+      </c>
+      <c r="F93" s="5" t="inlineStr">
+        <is>
+          <t>2.63</t>
+        </is>
+      </c>
+      <c r="G93" s="4" t="n">
+        <v>15722984.03440945</v>
+      </c>
+    </row>
+    <row r="94" ht="17" customHeight="1">
+      <c r="A94" s="3" t="inlineStr">
+        <is>
+          <t>NOG</t>
+        </is>
+      </c>
+      <c r="B94" s="6" t="n">
+        <v>24.03</v>
+      </c>
+      <c r="C94" s="7" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="D94" s="7" t="inlineStr">
+        <is>
+          <t>62.50</t>
+        </is>
+      </c>
+      <c r="E94" s="7" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="F94" s="7" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="G94" s="6" t="n">
+        <v>48729967.24078742</v>
+      </c>
+    </row>
+    <row r="95" ht="17" customHeight="1">
+      <c r="A95" s="3" t="inlineStr">
+        <is>
+          <t>NPKI</t>
+        </is>
+      </c>
+      <c r="B95" s="4" t="n">
+        <v>13.86</v>
+      </c>
+      <c r="C95" s="5" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="D95" s="5" t="inlineStr">
+        <is>
+          <t>61.06</t>
+        </is>
+      </c>
+      <c r="E95" s="5" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+      <c r="F95" s="5" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="G95" s="4" t="n">
+        <v>8826882.846062992</v>
+      </c>
+    </row>
+    <row r="96" ht="17" customHeight="1">
+      <c r="A96" s="3" t="inlineStr">
+        <is>
+          <t>NPO</t>
+        </is>
+      </c>
+      <c r="B96" s="6" t="n">
+        <v>238.26</v>
+      </c>
+      <c r="C96" s="7" t="inlineStr">
+        <is>
+          <t>1.43</t>
+        </is>
+      </c>
+      <c r="D96" s="7" t="inlineStr">
+        <is>
+          <t>57.78</t>
+        </is>
+      </c>
+      <c r="E96" s="7" t="inlineStr">
+        <is>
+          <t>4.90</t>
+        </is>
+      </c>
+      <c r="F96" s="7" t="inlineStr">
+        <is>
+          <t>4.21</t>
+        </is>
+      </c>
+      <c r="G96" s="6" t="n">
+        <v>36880755.52700788</v>
+      </c>
+    </row>
+    <row r="97" ht="17" customHeight="1">
+      <c r="A97" s="3" t="inlineStr">
+        <is>
+          <t>NRG</t>
+        </is>
+      </c>
+      <c r="B97" s="4" t="n">
+        <v>156.04</v>
+      </c>
+      <c r="C97" s="5" t="inlineStr">
+        <is>
+          <t>1.71</t>
+        </is>
+      </c>
+      <c r="D97" s="5" t="inlineStr">
+        <is>
+          <t>51.43</t>
+        </is>
+      </c>
+      <c r="E97" s="5" t="inlineStr">
+        <is>
+          <t>-2.35</t>
+        </is>
+      </c>
+      <c r="F97" s="5" t="inlineStr">
+        <is>
+          <t>-2.80</t>
+        </is>
+      </c>
+      <c r="G97" s="4" t="n">
+        <v>358124956.146378</v>
+      </c>
+    </row>
+    <row r="98" ht="17" customHeight="1">
+      <c r="A98" s="3" t="inlineStr">
+        <is>
+          <t>NVOX</t>
+        </is>
+      </c>
+      <c r="B98" s="6" t="n">
+        <v>32.38</v>
+      </c>
+      <c r="C98" s="7" t="inlineStr">
+        <is>
+          <t>1.75</t>
+        </is>
+      </c>
+      <c r="D98" s="7" t="inlineStr">
+        <is>
+          <t>64.40</t>
+        </is>
+      </c>
+      <c r="E98" s="7" t="inlineStr">
+        <is>
+          <t>2.62</t>
+        </is>
+      </c>
+      <c r="F98" s="7" t="inlineStr">
+        <is>
+          <t>2.12</t>
+        </is>
+      </c>
+      <c r="G98" s="6" t="n">
+        <v>47651150.6892126</v>
+      </c>
+    </row>
+    <row r="99" ht="17" customHeight="1">
+      <c r="A99" s="3" t="inlineStr">
+        <is>
+          <t>NVT</t>
+        </is>
+      </c>
+      <c r="B99" s="4" t="n">
+        <v>113.16</v>
+      </c>
+      <c r="C99" s="5" t="inlineStr">
+        <is>
+          <t>1.57</t>
+        </is>
+      </c>
+      <c r="D99" s="5" t="inlineStr">
+        <is>
+          <t>60.25</t>
+        </is>
+      </c>
+      <c r="E99" s="5" t="inlineStr">
+        <is>
+          <t>1.96</t>
+        </is>
+      </c>
+      <c r="F99" s="5" t="inlineStr">
+        <is>
+          <t>1.22</t>
+        </is>
+      </c>
+      <c r="G99" s="4" t="n">
+        <v>209226703.2994488</v>
+      </c>
+    </row>
+    <row r="100" ht="17" customHeight="1">
+      <c r="A100" s="3" t="inlineStr">
+        <is>
+          <t>NX</t>
+        </is>
+      </c>
+      <c r="B100" s="6" t="n">
+        <v>18.51</v>
+      </c>
+      <c r="C100" s="7" t="inlineStr">
+        <is>
+          <t>1.28</t>
+        </is>
+      </c>
+      <c r="D100" s="7" t="inlineStr">
+        <is>
+          <t>65.97</t>
+        </is>
+      </c>
+      <c r="E100" s="7" t="inlineStr">
+        <is>
+          <t>1.01</t>
+        </is>
+      </c>
+      <c r="F100" s="7" t="inlineStr">
+        <is>
+          <t>0.93</t>
+        </is>
+      </c>
+      <c r="G100" s="6" t="n">
+        <v>10727556.45866142</v>
+      </c>
+    </row>
+    <row r="101" ht="17" customHeight="1">
+      <c r="A101" s="3" t="inlineStr">
+        <is>
+          <t>OC</t>
+        </is>
+      </c>
+      <c r="B101" s="4" t="n">
+        <v>121.21</v>
+      </c>
+      <c r="C101" s="5" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+      <c r="D101" s="5" t="inlineStr">
+        <is>
+          <t>53.95</t>
+        </is>
+      </c>
+      <c r="E101" s="5" t="inlineStr">
+        <is>
+          <t>2.49</t>
+        </is>
+      </c>
+      <c r="F101" s="5" t="inlineStr">
+        <is>
+          <t>2.24</t>
+        </is>
+      </c>
+      <c r="G101" s="4" t="n">
+        <v>160185932.8866141</v>
+      </c>
+    </row>
+    <row r="102" ht="17" customHeight="1">
+      <c r="A102" s="3" t="inlineStr">
+        <is>
+          <t>OLN</t>
+        </is>
+      </c>
+      <c r="B102" s="6" t="n">
+        <v>22.87</v>
+      </c>
+      <c r="C102" s="7" t="inlineStr">
+        <is>
+          <t>1.84</t>
+        </is>
+      </c>
+      <c r="D102" s="7" t="inlineStr">
+        <is>
+          <t>52.05</t>
+        </is>
+      </c>
+      <c r="E102" s="7" t="inlineStr">
+        <is>
+          <t>0.66</t>
+        </is>
+      </c>
+      <c r="F102" s="7" t="inlineStr">
+        <is>
+          <t>0.62</t>
+        </is>
+      </c>
+      <c r="G102" s="6" t="n">
+        <v>58697241.91433071</v>
+      </c>
+    </row>
+    <row r="103" ht="17" customHeight="1">
+      <c r="A103" s="3" t="inlineStr">
+        <is>
+          <t>ONTO</t>
+        </is>
+      </c>
+      <c r="B103" s="4" t="n">
+        <v>208.46</v>
+      </c>
+      <c r="C103" s="5" t="inlineStr">
+        <is>
+          <t>2.29</t>
+        </is>
+      </c>
+      <c r="D103" s="5" t="inlineStr">
+        <is>
+          <t>67.37</t>
+        </is>
+      </c>
+      <c r="E103" s="5" t="inlineStr">
+        <is>
+          <t>14.32</t>
+        </is>
+      </c>
+      <c r="F103" s="5" t="inlineStr">
+        <is>
+          <t>13.67</t>
+        </is>
+      </c>
+      <c r="G103" s="4" t="n">
+        <v>150859836.7747244</v>
+      </c>
+    </row>
+    <row r="104" ht="17" customHeight="1">
+      <c r="A104" s="3" t="inlineStr">
+        <is>
+          <t>OSK</t>
+        </is>
+      </c>
+      <c r="B104" s="6" t="n">
+        <v>150.39</v>
+      </c>
+      <c r="C104" s="7" t="inlineStr">
+        <is>
+          <t>1.28</t>
+        </is>
+      </c>
+      <c r="D104" s="7" t="inlineStr">
+        <is>
+          <t>59.47</t>
+        </is>
+      </c>
+      <c r="E104" s="7" t="inlineStr">
+        <is>
+          <t>5.80</t>
+        </is>
+      </c>
+      <c r="F104" s="7" t="inlineStr">
+        <is>
+          <t>5.47</t>
+        </is>
+      </c>
+      <c r="G104" s="6" t="n">
+        <v>92978378.40960631</v>
+      </c>
+    </row>
+    <row r="105" ht="17" customHeight="1">
+      <c r="A105" s="3" t="inlineStr">
+        <is>
+          <t>OVV</t>
+        </is>
+      </c>
+      <c r="B105" s="4" t="n">
+        <v>42.77</v>
+      </c>
+      <c r="C105" s="5" t="inlineStr">
+        <is>
+          <t>1.44</t>
+        </is>
+      </c>
+      <c r="D105" s="5" t="inlineStr">
+        <is>
+          <t>66.95</t>
+        </is>
+      </c>
+      <c r="E105" s="5" t="inlineStr">
+        <is>
+          <t>0.65</t>
+        </is>
+      </c>
+      <c r="F105" s="5" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="G105" s="4" t="n">
+        <v>130257077.43</v>
+      </c>
+    </row>
+    <row r="106" ht="17" customHeight="1">
+      <c r="A106" s="3" t="inlineStr">
+        <is>
+          <t>PAM</t>
+        </is>
+      </c>
+      <c r="B106" s="6" t="n">
+        <v>89.23</v>
+      </c>
+      <c r="C106" s="7" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+      <c r="D106" s="7" t="inlineStr">
+        <is>
+          <t>62.42</t>
+        </is>
+      </c>
+      <c r="E106" s="7" t="inlineStr">
+        <is>
+          <t>-0.46</t>
+        </is>
+      </c>
+      <c r="F106" s="7" t="inlineStr">
+        <is>
+          <t>-1.03</t>
+        </is>
+      </c>
+      <c r="G106" s="6" t="n">
+        <v>22623987.23984252</v>
+      </c>
+    </row>
+    <row r="107" ht="17" customHeight="1">
+      <c r="A107" s="3" t="inlineStr">
+        <is>
+          <t>PBF</t>
+        </is>
+      </c>
+      <c r="B107" s="4" t="n">
+        <v>33.04</v>
+      </c>
+      <c r="C107" s="5" t="inlineStr">
+        <is>
+          <t>1.25</t>
+        </is>
+      </c>
+      <c r="D107" s="5" t="inlineStr">
+        <is>
+          <t>57.77</t>
+        </is>
+      </c>
+      <c r="E107" s="5" t="inlineStr">
+        <is>
+          <t>0.74</t>
+        </is>
+      </c>
+      <c r="F107" s="5" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="G107" s="4" t="n">
+        <v>97421827.9423622</v>
+      </c>
+    </row>
+    <row r="108" ht="17" customHeight="1">
+      <c r="A108" s="3" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
+      <c r="B108" s="6" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="C108" s="7" t="inlineStr">
+        <is>
+          <t>1.36</t>
+        </is>
+      </c>
+      <c r="D108" s="7" t="inlineStr">
+        <is>
+          <t>66.22</t>
+        </is>
+      </c>
+      <c r="E108" s="7" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+      <c r="F108" s="7" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="G108" s="6" t="n">
+        <v>149463627.0137008</v>
+      </c>
+    </row>
+    <row r="109" ht="17" customHeight="1">
+      <c r="A109" s="3" t="inlineStr">
+        <is>
+          <t>PRIM</t>
+        </is>
+      </c>
+      <c r="B109" s="4" t="n">
+        <v>151.94</v>
+      </c>
+      <c r="C109" s="5" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="D109" s="5" t="inlineStr">
+        <is>
+          <t>68.04</t>
+        </is>
+      </c>
+      <c r="E109" s="5" t="inlineStr">
+        <is>
+          <t>6.21</t>
+        </is>
+      </c>
+      <c r="F109" s="5" t="inlineStr">
+        <is>
+          <t>4.16</t>
+        </is>
+      </c>
+      <c r="G109" s="4" t="n">
+        <v>118075005.9773228</v>
+      </c>
+    </row>
+    <row r="110" ht="17" customHeight="1">
+      <c r="A110" s="3" t="inlineStr">
+        <is>
+          <t>PRSU</t>
+        </is>
+      </c>
+      <c r="B110" s="6" t="n">
+        <v>34.78</v>
+      </c>
+      <c r="C110" s="7" t="inlineStr">
+        <is>
+          <t>1.21</t>
+        </is>
+      </c>
+      <c r="D110" s="7" t="inlineStr">
+        <is>
+          <t>52.49</t>
+        </is>
+      </c>
+      <c r="E110" s="7" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="F110" s="7" t="inlineStr">
+        <is>
+          <t>-0.08</t>
+        </is>
+      </c>
+      <c r="G110" s="6" t="n">
+        <v>8234628.94055118</v>
+      </c>
+    </row>
+    <row r="111" ht="17" customHeight="1">
+      <c r="A111" s="3" t="inlineStr">
+        <is>
+          <t>PSTG</t>
+        </is>
+      </c>
+      <c r="B111" s="4" t="n">
+        <v>74.12</v>
+      </c>
+      <c r="C111" s="5" t="inlineStr">
+        <is>
+          <t>1.84</t>
+        </is>
+      </c>
+      <c r="D111" s="5" t="inlineStr">
+        <is>
+          <t>54.49</t>
+        </is>
+      </c>
+      <c r="E111" s="5" t="inlineStr">
+        <is>
+          <t>-0.14</t>
+        </is>
+      </c>
+      <c r="F111" s="5" t="inlineStr">
+        <is>
+          <t>-1.13</t>
+        </is>
+      </c>
+      <c r="G111" s="4" t="n">
+        <v>274117191.3470866</v>
+      </c>
+    </row>
+    <row r="112" ht="17" customHeight="1">
+      <c r="A112" s="3" t="inlineStr">
+        <is>
+          <t>PUMP</t>
+        </is>
+      </c>
+      <c r="B112" s="6" t="n">
+        <v>10.75</v>
+      </c>
+      <c r="C112" s="7" t="inlineStr">
+        <is>
+          <t>2.09</t>
+        </is>
+      </c>
+      <c r="D112" s="7" t="inlineStr">
+        <is>
+          <t>60.09</t>
+        </is>
+      </c>
+      <c r="E112" s="7" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+      <c r="F112" s="7" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
+      <c r="G112" s="6" t="n">
+        <v>22953205.28866142</v>
+      </c>
+    </row>
+    <row r="113" ht="17" customHeight="1">
+      <c r="A113" s="3" t="inlineStr">
+        <is>
+          <t>PWR</t>
+        </is>
+      </c>
+      <c r="B113" s="4" t="n">
+        <v>479.27</v>
+      </c>
+      <c r="C113" s="5" t="inlineStr">
+        <is>
+          <t>1.21</t>
+        </is>
+      </c>
+      <c r="D113" s="5" t="inlineStr">
+        <is>
+          <t>65.22</t>
+        </is>
+      </c>
+      <c r="E113" s="5" t="inlineStr">
+        <is>
+          <t>9.60</t>
+        </is>
+      </c>
+      <c r="F113" s="5" t="inlineStr">
+        <is>
+          <t>4.01</t>
+        </is>
+      </c>
+      <c r="G113" s="4" t="n">
+        <v>431504166.8977166</v>
+      </c>
+    </row>
+    <row r="114" ht="17" customHeight="1">
+      <c r="A114" s="3" t="inlineStr">
+        <is>
+          <t>PX</t>
+        </is>
+      </c>
+      <c r="B114" s="6" t="n">
+        <v>10.97</v>
+      </c>
+      <c r="C114" s="7" t="inlineStr">
+        <is>
+          <t>1.32</t>
+        </is>
+      </c>
+      <c r="D114" s="7" t="inlineStr">
+        <is>
+          <t>61.75</t>
+        </is>
+      </c>
+      <c r="E114" s="7" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="F114" s="7" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="G114" s="6" t="n">
+        <v>5061290.032047245</v>
+      </c>
+    </row>
+    <row r="115" ht="17" customHeight="1">
+      <c r="A115" s="3" t="inlineStr">
+        <is>
+          <t>RCUS</t>
+        </is>
+      </c>
+      <c r="B115" s="4" t="n">
+        <v>22.99</v>
+      </c>
+      <c r="C115" s="5" t="inlineStr">
+        <is>
+          <t>1.33</t>
+        </is>
+      </c>
+      <c r="D115" s="5" t="inlineStr">
+        <is>
+          <t>52.33</t>
+        </is>
+      </c>
+      <c r="E115" s="5" t="inlineStr">
+        <is>
+          <t>-0.01</t>
+        </is>
+      </c>
+      <c r="F115" s="5" t="inlineStr">
+        <is>
+          <t>-0.03</t>
+        </is>
+      </c>
+      <c r="G115" s="4" t="n">
+        <v>26900790.15456693</v>
+      </c>
+    </row>
+    <row r="116" ht="17" customHeight="1">
+      <c r="A116" s="3" t="inlineStr">
+        <is>
+          <t>RDW</t>
+        </is>
+      </c>
+      <c r="B116" s="6" t="n">
+        <v>14.2</v>
+      </c>
+      <c r="C116" s="7" t="inlineStr">
+        <is>
+          <t>2.70</t>
+        </is>
+      </c>
+      <c r="D116" s="7" t="inlineStr">
+        <is>
+          <t>67.68</t>
+        </is>
+      </c>
+      <c r="E116" s="7" t="inlineStr">
+        <is>
+          <t>1.24</t>
+        </is>
+      </c>
+      <c r="F116" s="7" t="inlineStr">
+        <is>
+          <t>1.01</t>
+        </is>
+      </c>
+      <c r="G116" s="6" t="n">
+        <v>106590768.2738583</v>
+      </c>
+    </row>
+    <row r="117" ht="17" customHeight="1">
+      <c r="A117" s="3" t="inlineStr">
+        <is>
+          <t>RXO</t>
+        </is>
+      </c>
+      <c r="B117" s="4" t="n">
+        <v>14.53</v>
+      </c>
+      <c r="C117" s="5" t="inlineStr">
+        <is>
+          <t>2.00</t>
+        </is>
+      </c>
+      <c r="D117" s="5" t="inlineStr">
+        <is>
+          <t>50.09</t>
+        </is>
+      </c>
+      <c r="E117" s="5" t="inlineStr">
+        <is>
+          <t>0.39</t>
+        </is>
+      </c>
+      <c r="F117" s="5" t="inlineStr">
+        <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="G117" s="4" t="n">
+        <v>30849841.0276378</v>
+      </c>
+    </row>
+    <row r="118" ht="17" customHeight="1">
+      <c r="A118" s="3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="B118" s="6" t="n">
+        <v>15.11</v>
+      </c>
+      <c r="C118" s="7" t="inlineStr">
+        <is>
+          <t>1.39</t>
+        </is>
+      </c>
+      <c r="D118" s="7" t="inlineStr">
+        <is>
+          <t>55.05</t>
+        </is>
+      </c>
+      <c r="E118" s="7" t="inlineStr">
+        <is>
+          <t>-0.24</t>
+        </is>
+      </c>
+      <c r="F118" s="7" t="inlineStr">
+        <is>
+          <t>-0.31</t>
+        </is>
+      </c>
+      <c r="G118" s="6" t="n">
+        <v>116455878.0688189</v>
+      </c>
+    </row>
+    <row r="119" ht="17" customHeight="1">
+      <c r="A119" s="3" t="inlineStr">
+        <is>
+          <t>SDRL</t>
+        </is>
+      </c>
+      <c r="B119" s="4" t="n">
+        <v>38.75</v>
+      </c>
+      <c r="C119" s="5" t="inlineStr">
+        <is>
+          <t>1.42</t>
+        </is>
+      </c>
+      <c r="D119" s="5" t="inlineStr">
+        <is>
+          <t>67.98</t>
+        </is>
+      </c>
+      <c r="E119" s="5" t="inlineStr">
+        <is>
+          <t>1.59</t>
+        </is>
+      </c>
+      <c r="F119" s="5" t="inlineStr">
+        <is>
+          <t>1.15</t>
+        </is>
+      </c>
+      <c r="G119" s="4" t="n">
+        <v>25710150.84858268</v>
+      </c>
+    </row>
+    <row r="120" ht="17" customHeight="1">
+      <c r="A120" s="3" t="inlineStr">
+        <is>
+          <t>SEI</t>
+        </is>
+      </c>
+      <c r="B120" s="6" t="n">
+        <v>53.9</v>
+      </c>
+      <c r="C120" s="7" t="inlineStr">
+        <is>
+          <t>2.23</t>
+        </is>
+      </c>
+      <c r="D120" s="7" t="inlineStr">
+        <is>
+          <t>54.81</t>
+        </is>
+      </c>
+      <c r="E120" s="7" t="inlineStr">
+        <is>
+          <t>1.71</t>
+        </is>
+      </c>
+      <c r="F120" s="7" t="inlineStr">
+        <is>
+          <t>1.57</t>
+        </is>
+      </c>
+      <c r="G120" s="6" t="n">
+        <v>133042488.256063</v>
+      </c>
+    </row>
+    <row r="121" ht="17" customHeight="1">
+      <c r="A121" s="3" t="inlineStr">
+        <is>
+          <t>SES</t>
+        </is>
+      </c>
+      <c r="B121" s="4" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="C121" s="5" t="inlineStr">
+        <is>
+          <t>1.72</t>
+        </is>
+      </c>
+      <c r="D121" s="5" t="inlineStr">
+        <is>
+          <t>51.32</t>
+        </is>
+      </c>
+      <c r="E121" s="5" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="F121" s="5" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="G121" s="4" t="n">
+        <v>24511913.44968504</v>
+      </c>
+    </row>
+    <row r="122" ht="17" customHeight="1">
+      <c r="A122" s="3" t="inlineStr">
+        <is>
+          <t>SHCO</t>
+        </is>
+      </c>
+      <c r="B122" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C122" s="7" t="inlineStr">
+        <is>
+          <t>1.44</t>
+        </is>
+      </c>
+      <c r="D122" s="7" t="inlineStr">
+        <is>
+          <t>60.00</t>
+        </is>
+      </c>
+      <c r="E122" s="7" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="F122" s="7" t="inlineStr">
+        <is>
+          <t>-0.05</t>
+        </is>
+      </c>
+      <c r="G122" s="6" t="n">
+        <v>9384485.76</v>
+      </c>
+    </row>
+    <row r="123" ht="17" customHeight="1">
+      <c r="A123" s="3" t="inlineStr">
+        <is>
+          <t>SIG</t>
+        </is>
+      </c>
+      <c r="B123" s="4" t="n">
+        <v>90.56</v>
+      </c>
+      <c r="C123" s="5" t="inlineStr">
+        <is>
+          <t>1.53</t>
+        </is>
+      </c>
+      <c r="D123" s="5" t="inlineStr">
+        <is>
+          <t>51.15</t>
+        </is>
+      </c>
+      <c r="E123" s="5" t="inlineStr">
+        <is>
+          <t>0.69</t>
+        </is>
+      </c>
+      <c r="F123" s="5" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="G123" s="4" t="n">
+        <v>80215668.05393703</v>
+      </c>
+    </row>
+    <row r="124" ht="17" customHeight="1">
+      <c r="A124" s="3" t="inlineStr">
+        <is>
+          <t>SM</t>
+        </is>
+      </c>
+      <c r="B124" s="6" t="n">
+        <v>19.28</v>
+      </c>
+      <c r="C124" s="7" t="inlineStr">
+        <is>
+          <t>1.68</t>
+        </is>
+      </c>
+      <c r="D124" s="7" t="inlineStr">
+        <is>
+          <t>57.00</t>
+        </is>
+      </c>
+      <c r="E124" s="7" t="inlineStr">
+        <is>
+          <t>-0.02</t>
+        </is>
+      </c>
+      <c r="F124" s="7" t="inlineStr">
+        <is>
+          <t>-0.20</t>
+        </is>
+      </c>
+      <c r="G124" s="6" t="n">
+        <v>58427808.18850394</v>
+      </c>
+    </row>
+    <row r="125" ht="17" customHeight="1">
+      <c r="A125" s="3" t="inlineStr">
+        <is>
+          <t>SSTK</t>
+        </is>
+      </c>
+      <c r="B125" s="4" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="C125" s="5" t="inlineStr">
+        <is>
+          <t>1.38</t>
+        </is>
+      </c>
+      <c r="D125" s="5" t="inlineStr">
+        <is>
+          <t>58.21</t>
+        </is>
+      </c>
+      <c r="E125" s="5" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="F125" s="5" t="inlineStr">
+        <is>
+          <t>-0.20</t>
+        </is>
+      </c>
+      <c r="G125" s="4" t="n">
+        <v>5544149.576220474</v>
+      </c>
+    </row>
+    <row r="126" ht="17" customHeight="1">
+      <c r="A126" s="3" t="inlineStr">
+        <is>
+          <t>STM</t>
+        </is>
+      </c>
+      <c r="B126" s="6" t="n">
+        <v>29.36</v>
+      </c>
+      <c r="C126" s="7" t="inlineStr">
+        <is>
+          <t>1.83</t>
+        </is>
+      </c>
+      <c r="D126" s="7" t="inlineStr">
+        <is>
+          <t>63.21</t>
+        </is>
+      </c>
+      <c r="E126" s="7" t="inlineStr">
+        <is>
+          <t>0.76</t>
+        </is>
+      </c>
+      <c r="F126" s="7" t="inlineStr">
+        <is>
+          <t>0.73</t>
+        </is>
+      </c>
+      <c r="G126" s="6" t="n">
+        <v>161497139.6877165</v>
+      </c>
+    </row>
+    <row r="127" ht="17" customHeight="1">
+      <c r="A127" s="3" t="inlineStr">
+        <is>
+          <t>SUPV</t>
+        </is>
+      </c>
+      <c r="B127" s="4" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="C127" s="5" t="inlineStr">
+        <is>
+          <t>1.76</t>
+        </is>
+      </c>
+      <c r="D127" s="5" t="inlineStr">
+        <is>
+          <t>60.06</t>
+        </is>
+      </c>
+      <c r="E127" s="5" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="F127" s="5" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="G127" s="4" t="n">
+        <v>17928483.55685039</v>
+      </c>
+    </row>
+    <row r="128" ht="17" customHeight="1">
+      <c r="A128" s="3" t="inlineStr">
+        <is>
+          <t>SW</t>
+        </is>
+      </c>
+      <c r="B128" s="6" t="n">
+        <v>42.96</v>
+      </c>
+      <c r="C128" s="7" t="inlineStr">
+        <is>
+          <t>1.26</t>
+        </is>
+      </c>
+      <c r="D128" s="7" t="inlineStr">
+        <is>
+          <t>60.76</t>
+        </is>
+      </c>
+      <c r="E128" s="7" t="inlineStr">
+        <is>
+          <t>1.27</t>
+        </is>
+      </c>
+      <c r="F128" s="7" t="inlineStr">
+        <is>
+          <t>1.24</t>
+        </is>
+      </c>
+      <c r="G128" s="6" t="n">
+        <v>197945036.212126</v>
+      </c>
+    </row>
+    <row r="129" ht="17" customHeight="1">
+      <c r="A129" s="3" t="inlineStr">
+        <is>
+          <t>TALO</t>
+        </is>
+      </c>
+      <c r="B129" s="4" t="n">
+        <v>11.73</v>
+      </c>
+      <c r="C129" s="5" t="inlineStr">
+        <is>
+          <t>1.50</t>
+        </is>
+      </c>
+      <c r="D129" s="5" t="inlineStr">
+        <is>
+          <t>58.02</t>
+        </is>
+      </c>
+      <c r="E129" s="5" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="F129" s="5" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="G129" s="4" t="n">
+        <v>20793385.27716535</v>
+      </c>
+    </row>
+    <row r="130" ht="17" customHeight="1">
+      <c r="A130" s="3" t="inlineStr">
+        <is>
+          <t>TKR</t>
+        </is>
+      </c>
+      <c r="B130" s="6" t="n">
+        <v>93.89</v>
+      </c>
+      <c r="C130" s="7" t="inlineStr">
+        <is>
+          <t>1.27</t>
+        </is>
+      </c>
+      <c r="D130" s="7" t="inlineStr">
+        <is>
+          <t>63.39</t>
+        </is>
+      </c>
+      <c r="E130" s="7" t="inlineStr">
+        <is>
+          <t>2.47</t>
+        </is>
+      </c>
+      <c r="F130" s="7" t="inlineStr">
+        <is>
+          <t>2.37</t>
+        </is>
+      </c>
+      <c r="G130" s="6" t="n">
+        <v>53529899.01669293</v>
+      </c>
+    </row>
+    <row r="131" ht="17" customHeight="1">
+      <c r="A131" s="3" t="inlineStr">
+        <is>
+          <t>TPL</t>
+        </is>
+      </c>
+      <c r="B131" s="4" t="n">
+        <v>345.2</v>
+      </c>
+      <c r="C131" s="5" t="inlineStr">
+        <is>
+          <t>1.35</t>
+        </is>
+      </c>
+      <c r="D131" s="5" t="inlineStr">
+        <is>
+          <t>65.39</t>
+        </is>
+      </c>
+      <c r="E131" s="5" t="inlineStr">
+        <is>
+          <t>12.84</t>
+        </is>
+      </c>
+      <c r="F131" s="5" t="inlineStr">
+        <is>
+          <t>8.14</t>
+        </is>
+      </c>
+      <c r="G131" s="4" t="n">
+        <v>124452291.6852362</v>
+      </c>
+    </row>
+    <row r="132" ht="17" customHeight="1">
+      <c r="A132" s="3" t="inlineStr">
+        <is>
+          <t>TREX</t>
+        </is>
+      </c>
+      <c r="B132" s="6" t="n">
+        <v>41.91</v>
+      </c>
+      <c r="C132" s="7" t="inlineStr">
+        <is>
+          <t>1.27</t>
+        </is>
+      </c>
+      <c r="D132" s="7" t="inlineStr">
+        <is>
+          <t>60.78</t>
+        </is>
+      </c>
+      <c r="E132" s="7" t="inlineStr">
+        <is>
+          <t>1.74</t>
+        </is>
+      </c>
+      <c r="F132" s="7" t="inlineStr">
+        <is>
+          <t>1.50</t>
+        </is>
+      </c>
+      <c r="G132" s="6" t="n">
+        <v>98972166.46015748</v>
+      </c>
+    </row>
+    <row r="133" ht="17" customHeight="1">
+      <c r="A133" s="3" t="inlineStr">
+        <is>
+          <t>TSM</t>
+        </is>
+      </c>
+      <c r="B133" s="4" t="n">
+        <v>338.34</v>
+      </c>
+      <c r="C133" s="5" t="inlineStr">
+        <is>
+          <t>1.49</t>
+        </is>
+      </c>
+      <c r="D133" s="5" t="inlineStr">
+        <is>
+          <t>63.51</t>
+        </is>
+      </c>
+      <c r="E133" s="5" t="inlineStr">
+        <is>
+          <t>9.16</t>
+        </is>
+      </c>
+      <c r="F133" s="5" t="inlineStr">
+        <is>
+          <t>8.92</t>
+        </is>
+      </c>
+      <c r="G133" s="4" t="n">
+        <v>3553642038.131731</v>
+      </c>
+    </row>
+    <row r="134" ht="17" customHeight="1">
+      <c r="A134" s="3" t="inlineStr">
+        <is>
+          <t>TTI</t>
+        </is>
+      </c>
+      <c r="B134" s="6" t="n">
+        <v>11.92</v>
+      </c>
+      <c r="C134" s="7" t="inlineStr">
+        <is>
+          <t>1.51</t>
+        </is>
+      </c>
+      <c r="D134" s="7" t="inlineStr">
+        <is>
+          <t>69.99</t>
+        </is>
+      </c>
+      <c r="E134" s="7" t="inlineStr">
+        <is>
+          <t>0.75</t>
+        </is>
+      </c>
+      <c r="F134" s="7" t="inlineStr">
+        <is>
+          <t>0.67</t>
+        </is>
+      </c>
+      <c r="G134" s="6" t="n">
+        <v>16246705.53251969</v>
+      </c>
+    </row>
+    <row r="135" ht="17" customHeight="1">
+      <c r="A135" s="3" t="inlineStr">
+        <is>
+          <t>VAL</t>
+        </is>
+      </c>
+      <c r="B135" s="4" t="n">
+        <v>58.29</v>
+      </c>
+      <c r="C135" s="5" t="inlineStr">
+        <is>
+          <t>1.57</t>
+        </is>
+      </c>
+      <c r="D135" s="5" t="inlineStr">
+        <is>
+          <t>68.37</t>
+        </is>
+      </c>
+      <c r="E135" s="5" t="inlineStr">
+        <is>
+          <t>0.92</t>
+        </is>
+      </c>
+      <c r="F135" s="5" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="G135" s="4" t="n">
+        <v>58660116.02700789</v>
+      </c>
+    </row>
+    <row r="136" ht="17" customHeight="1">
+      <c r="A136" s="3" t="inlineStr">
+        <is>
+          <t>VET</t>
+        </is>
+      </c>
+      <c r="B136" s="6" t="n">
+        <v>9.69</v>
+      </c>
+      <c r="C136" s="7" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
+      <c r="D136" s="7" t="inlineStr">
+        <is>
+          <t>66.81</t>
+        </is>
+      </c>
+      <c r="E136" s="7" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="F136" s="7" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="G136" s="6" t="n">
+        <v>10191463.99425197</v>
+      </c>
+    </row>
+    <row r="137" ht="17" customHeight="1">
+      <c r="A137" s="3" t="inlineStr">
+        <is>
+          <t>VFC</t>
+        </is>
+      </c>
+      <c r="B137" s="4" t="n">
+        <v>20.28</v>
+      </c>
+      <c r="C137" s="5" t="inlineStr">
+        <is>
+          <t>2.46</t>
+        </is>
+      </c>
+      <c r="D137" s="5" t="inlineStr">
+        <is>
+          <t>63.52</t>
+        </is>
+      </c>
+      <c r="E137" s="5" t="inlineStr">
+        <is>
+          <t>0.46</t>
+        </is>
+      </c>
+      <c r="F137" s="5" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="G137" s="4" t="n">
+        <v>114983720.5869291</v>
+      </c>
+    </row>
+    <row r="138" ht="17" customHeight="1">
+      <c r="A138" s="3" t="inlineStr">
+        <is>
+          <t>VG</t>
+        </is>
+      </c>
+      <c r="B138" s="6" t="n">
+        <v>8.91</v>
+      </c>
+      <c r="C138" s="7" t="inlineStr">
+        <is>
+          <t>1.80</t>
+        </is>
+      </c>
+      <c r="D138" s="7" t="inlineStr">
+        <is>
+          <t>60.43</t>
+        </is>
+      </c>
+      <c r="E138" s="7" t="inlineStr">
+        <is>
+          <t>0.61</t>
+        </is>
+      </c>
+      <c r="F138" s="7" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+      <c r="G138" s="6" t="n">
+        <v>96583077.94511808</v>
+      </c>
+    </row>
+    <row r="139" ht="17" customHeight="1">
+      <c r="A139" s="3" t="inlineStr">
+        <is>
+          <t>VPG</t>
+        </is>
+      </c>
+      <c r="B139" s="4" t="n">
+        <v>44.98</v>
+      </c>
+      <c r="C139" s="5" t="inlineStr">
+        <is>
+          <t>1.82</t>
+        </is>
+      </c>
+      <c r="D139" s="5" t="inlineStr">
+        <is>
+          <t>61.61</t>
+        </is>
+      </c>
+      <c r="E139" s="5" t="inlineStr">
+        <is>
+          <t>1.88</t>
+        </is>
+      </c>
+      <c r="F139" s="5" t="inlineStr">
+        <is>
+          <t>1.71</t>
+        </is>
+      </c>
+      <c r="G139" s="4" t="n">
+        <v>5145228.372992126</v>
+      </c>
+    </row>
+    <row r="140" ht="17" customHeight="1">
+      <c r="A140" s="3" t="inlineStr">
+        <is>
+          <t>VRT</t>
+        </is>
+      </c>
+      <c r="B140" s="6" t="n">
+        <v>189.21</v>
+      </c>
+      <c r="C140" s="7" t="inlineStr">
+        <is>
+          <t>2.25</t>
+        </is>
+      </c>
+      <c r="D140" s="7" t="inlineStr">
+        <is>
+          <t>65.09</t>
+        </is>
+      </c>
+      <c r="E140" s="7" t="inlineStr">
+        <is>
+          <t>3.83</t>
+        </is>
+      </c>
+      <c r="F140" s="7" t="inlineStr">
+        <is>
+          <t>1.47</t>
+        </is>
+      </c>
+      <c r="G140" s="6" t="n">
+        <v>1116583470.738898</v>
+      </c>
+    </row>
+    <row r="141" ht="17" customHeight="1">
+      <c r="A141" s="3" t="inlineStr">
+        <is>
+          <t>VSH</t>
+        </is>
+      </c>
+      <c r="B141" s="4" t="n">
+        <v>18.48</v>
+      </c>
+      <c r="C141" s="5" t="inlineStr">
+        <is>
+          <t>2.14</t>
+        </is>
+      </c>
+      <c r="D141" s="5" t="inlineStr">
+        <is>
+          <t>65.84</t>
+        </is>
+      </c>
+      <c r="E141" s="5" t="inlineStr">
+        <is>
+          <t>0.94</t>
+        </is>
+      </c>
+      <c r="F141" s="5" t="inlineStr">
+        <is>
+          <t>0.72</t>
+        </is>
+      </c>
+      <c r="G141" s="4" t="n">
+        <v>26557856.71527559</v>
+      </c>
+    </row>
+    <row r="142" ht="17" customHeight="1">
+      <c r="A142" s="3" t="inlineStr">
+        <is>
+          <t>WCC</t>
+        </is>
+      </c>
+      <c r="B142" s="6" t="n">
+        <v>287.81</v>
+      </c>
+      <c r="C142" s="7" t="inlineStr">
+        <is>
+          <t>1.58</t>
+        </is>
+      </c>
+      <c r="D142" s="7" t="inlineStr">
+        <is>
+          <t>63.89</t>
+        </is>
+      </c>
+      <c r="E142" s="7" t="inlineStr">
+        <is>
+          <t>7.88</t>
+        </is>
+      </c>
+      <c r="F142" s="7" t="inlineStr">
+        <is>
+          <t>5.90</t>
+        </is>
+      </c>
+      <c r="G142" s="6" t="n">
+        <v>137907492.5231496</v>
+      </c>
+    </row>
+    <row r="143" ht="17" customHeight="1">
+      <c r="A143" s="3" t="inlineStr">
+        <is>
+          <t>WGO</t>
+        </is>
+      </c>
+      <c r="B143" s="4" t="n">
+        <v>46.81</v>
+      </c>
+      <c r="C143" s="5" t="inlineStr">
+        <is>
+          <t>1.28</t>
+        </is>
+      </c>
+      <c r="D143" s="5" t="inlineStr">
+        <is>
+          <t>61.37</t>
+        </is>
+      </c>
+      <c r="E143" s="5" t="inlineStr">
+        <is>
+          <t>1.93</t>
+        </is>
+      </c>
+      <c r="F143" s="5" t="inlineStr">
+        <is>
+          <t>1.90</t>
+        </is>
+      </c>
+      <c r="G143" s="4" t="n">
+        <v>22564818.40409449</v>
+      </c>
+    </row>
+    <row r="144" ht="17" customHeight="1">
+      <c r="A144" s="3" t="inlineStr">
+        <is>
+          <t>WS</t>
+        </is>
+      </c>
+      <c r="B144" s="6" t="n">
+        <v>38.95</v>
+      </c>
+      <c r="C144" s="7" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
+      </c>
+      <c r="D144" s="7" t="inlineStr">
+        <is>
+          <t>60.81</t>
+        </is>
+      </c>
+      <c r="E144" s="7" t="inlineStr">
+        <is>
+          <t>1.21</t>
+        </is>
+      </c>
+      <c r="F144" s="7" t="inlineStr">
+        <is>
+          <t>1.03</t>
+        </is>
+      </c>
+      <c r="G144" s="6" t="n">
+        <v>8232046.139527558</v>
+      </c>
+    </row>
+    <row r="145" ht="17" customHeight="1">
+      <c r="A145" s="3" t="inlineStr">
+        <is>
+          <t>WSM</t>
+        </is>
+      </c>
+      <c r="B145" s="4" t="n">
+        <v>208.25</v>
+      </c>
+      <c r="C145" s="5" t="inlineStr">
+        <is>
+          <t>1.40</t>
+        </is>
+      </c>
+      <c r="D145" s="5" t="inlineStr">
+        <is>
+          <t>58.90</t>
+        </is>
+      </c>
+      <c r="E145" s="5" t="inlineStr">
+        <is>
+          <t>5.55</t>
+        </is>
+      </c>
+      <c r="F145" s="5" t="inlineStr">
+        <is>
+          <t>5.13</t>
+        </is>
+      </c>
+      <c r="G145" s="4" t="n">
+        <v>234774867.4489764</v>
+      </c>
+    </row>
+    <row r="146" ht="17" customHeight="1">
+      <c r="A146" s="3" t="inlineStr">
+        <is>
+          <t>WTTR</t>
+        </is>
+      </c>
+      <c r="B146" s="6" t="n">
+        <v>11.74</v>
+      </c>
+      <c r="C146" s="7" t="inlineStr">
+        <is>
+          <t>1.26</t>
+        </is>
+      </c>
+      <c r="D146" s="7" t="inlineStr">
+        <is>
+          <t>55.98</t>
+        </is>
+      </c>
+      <c r="E146" s="7" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="F146" s="7" t="inlineStr">
+        <is>
+          <t>0.26</t>
+        </is>
+      </c>
+      <c r="G146" s="6" t="n">
+        <v>9923063.715590551</v>
+      </c>
+    </row>
+    <row r="147" ht="17" customHeight="1">
+      <c r="A147" s="3" t="inlineStr">
+        <is>
+          <t>XPRO</t>
+        </is>
+      </c>
+      <c r="B147" s="4" t="n">
+        <v>16.08</v>
+      </c>
+      <c r="C147" s="5" t="inlineStr">
+        <is>
+          <t>1.69</t>
+        </is>
+      </c>
+      <c r="D147" s="5" t="inlineStr">
+        <is>
+          <t>63.17</t>
+        </is>
+      </c>
+      <c r="E147" s="5" t="inlineStr">
+        <is>
+          <t>0.61</t>
+        </is>
+      </c>
+      <c r="F147" s="5" t="inlineStr">
+        <is>
+          <t>0.47</t>
+        </is>
+      </c>
+      <c r="G147" s="4" t="n">
+        <v>15867501.62850394</v>
+      </c>
+    </row>
+    <row r="148" ht="17" customHeight="1">
+      <c r="A148" s="3" t="inlineStr">
+        <is>
+          <t>YPF</t>
+        </is>
+      </c>
+      <c r="B148" s="6" t="n">
+        <v>38.28</v>
+      </c>
+      <c r="C148" s="7" t="inlineStr">
+        <is>
+          <t>1.22</t>
+        </is>
+      </c>
+      <c r="D148" s="7" t="inlineStr">
+        <is>
+          <t>66.10</t>
+        </is>
+      </c>
+      <c r="E148" s="7" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+      <c r="F148" s="7" t="inlineStr">
+        <is>
+          <t>-0.04</t>
+        </is>
+      </c>
+      <c r="G148" s="6" t="n">
+        <v>70116180.81141731</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>